<commit_message>
Latest code for Workday UFT to Playwright Migration
</commit_message>
<xml_diff>
--- a/Data/testDataRomania.xlsx
+++ b/Data/testDataRomania.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{785EEA98-F72F-4EF5-94F5-E1291935D67D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{EAAAFB97-0E2B-4641-86BC-642FD18F8C83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,6 +11,7 @@
     <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -264,7 +265,7 @@
     <t>Test1</t>
   </si>
   <si>
-    <t xml:space="preserve">Test failed for 'Ursula Sporer' Employee: Errors and AlertsErrorsNational IDs (Row 1)Enter a National ID in the valid format: six digits onlyNational IDs (Row 2)Enter a National ID in the valid format: thirteen digits only </t>
+    <t>{"name":"TimeoutError"}</t>
   </si>
   <si>
     <t>Failed</t>
@@ -276,10 +277,10 @@
     <t>Romania</t>
   </si>
   <si>
-    <t>Ursula</t>
-  </si>
-  <si>
-    <t>Sporer</t>
+    <t>Suzanne</t>
+  </si>
+  <si>
+    <t>Reichel</t>
   </si>
   <si>
     <t>Mobile</t>
@@ -571,7 +572,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -653,11 +654,20 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="15" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -940,8 +950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CD4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.65" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1445,7 +1455,7 @@
         <v>111</v>
       </c>
       <c r="BD2" s="28">
-        <v>1910411415830</v>
+        <v>1760728315979</v>
       </c>
       <c r="BE2" s="21" t="s">
         <v>112</v>
@@ -1460,7 +1470,7 @@
         <v>114</v>
       </c>
       <c r="BI2" s="29">
-        <v>212481</v>
+        <v>212484</v>
       </c>
       <c r="BJ2" s="17" t="s">
         <v>112</v>
@@ -1477,25 +1487,25 @@
       <c r="BN2" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="BO2" s="30" t="s">
+      <c r="BO2" s="34" t="s">
         <v>116</v>
       </c>
-      <c r="BP2" s="17" t="s">
+      <c r="BP2" s="35" t="s">
         <v>117</v>
       </c>
-      <c r="BQ2" s="31" t="s">
+      <c r="BQ2" s="36" t="s">
         <v>89</v>
       </c>
-      <c r="BR2" s="20" t="s">
+      <c r="BR2" s="37" t="s">
         <v>118</v>
       </c>
-      <c r="BS2" s="32" t="s">
+      <c r="BS2" s="38" t="s">
         <v>100</v>
       </c>
-      <c r="BT2" s="16" t="s">
+      <c r="BT2" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="BU2" s="16" t="s">
+      <c r="BU2" s="26" t="s">
         <v>81</v>
       </c>
       <c r="BV2" s="30" t="s">
@@ -1530,7 +1540,7 @@
       <c r="A3" t="s">
         <v>127</v>
       </c>
-      <c r="B3" s="33"/>
+      <c r="B3" s="32"/>
       <c r="C3" s="8" t="s">
         <v>79</v>
       </c>
@@ -1671,7 +1681,7 @@
       <c r="AV3" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="AW3" s="34" t="s">
+      <c r="AW3" s="33" t="s">
         <v>134</v>
       </c>
       <c r="AX3" s="15" t="s">
@@ -1728,25 +1738,25 @@
       <c r="BN3" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="BO3" s="30" t="s">
+      <c r="BO3" s="34" t="s">
         <v>116</v>
       </c>
-      <c r="BP3" s="17" t="s">
+      <c r="BP3" s="35" t="s">
         <v>117</v>
       </c>
-      <c r="BQ3" s="31" t="s">
+      <c r="BQ3" s="36" t="s">
         <v>89</v>
       </c>
-      <c r="BR3" s="20" t="s">
+      <c r="BR3" s="37" t="s">
         <v>118</v>
       </c>
-      <c r="BS3" s="32" t="s">
+      <c r="BS3" s="38" t="s">
         <v>100</v>
       </c>
-      <c r="BT3" s="16" t="s">
+      <c r="BT3" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="BU3" s="16" t="s">
+      <c r="BU3" s="26" t="s">
         <v>81</v>
       </c>
       <c r="BV3" s="30" t="s">

</xml_diff>

<commit_message>
Latest code for Romania migration testcase
</commit_message>
<xml_diff>
--- a/Data/testDataRomania.xlsx
+++ b/Data/testDataRomania.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="139">
   <si>
     <t>TestCaseIDs</t>
   </si>
@@ -262,10 +262,10 @@
     <t>Romania</t>
   </si>
   <si>
-    <t>EtwoETwentyTWOf</t>
-  </si>
-  <si>
-    <t>HireBatchOne</t>
+    <t>Elias</t>
+  </si>
+  <si>
+    <t>Simonis</t>
   </si>
   <si>
     <t>Mobile</t>
@@ -298,7 +298,7 @@
     <t>No</t>
   </si>
   <si>
-    <t>Fixed Term</t>
+    <t>Fixed Term (Fixed Term)</t>
   </si>
   <si>
     <t>In-Store P&amp;C Assistant_NEW</t>
@@ -407,22 +407,31 @@
     <t>Test3</t>
   </si>
   <si>
-    <t>10650585</t>
-  </si>
-  <si>
-    <t>EtwoETwentyEIGHTz</t>
-  </si>
-  <si>
-    <t>Visual Merchandiser_NEW</t>
+    <t>10650771</t>
+  </si>
+  <si>
+    <t>880 Store Management (Dewes Kiwoba (10629083))</t>
+  </si>
+  <si>
+    <t>Jorge</t>
+  </si>
+  <si>
+    <t>Nikolaus</t>
+  </si>
+  <si>
+    <t>Auto 70059278</t>
+  </si>
+  <si>
+    <t>Team Manager - Retail_NEW</t>
   </si>
   <si>
     <t>Part Time</t>
   </si>
   <si>
-    <t>256 Visual Merchandising</t>
-  </si>
-  <si>
-    <t>436329</t>
+    <t xml:space="preserve">92 Retail Management </t>
+  </si>
+  <si>
+    <t>251 Management Retail</t>
   </si>
 </sst>
 </file>
@@ -432,7 +441,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <color theme="1"/>
       <family val="2"/>
@@ -467,8 +476,15 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <color rgb="FF000000"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -496,6 +512,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00FF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF01"/>
       </patternFill>
     </fill>
   </fills>
@@ -542,7 +563,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -602,7 +623,7 @@
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -638,15 +659,21 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -944,7 +971,7 @@
   <dimension ref="A1:CD32"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="BI3" sqref="BI3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.65" outlineLevelRow="1" outlineLevelCol="0" x14ac:dyDescent="0.35" customHeight="1"/>
@@ -1313,7 +1340,7 @@
       </c>
       <c r="K2" s="16" t="str">
         <f t="shared" ref="K2" si="0">TEXT(TODAY()-100,"DD/MM/YYYY")</f>
-        <v>29/06/2024</v>
+        <v>01/07/2024</v>
       </c>
       <c r="L2" s="13" t="s">
         <v>81</v>
@@ -1350,7 +1377,7 @@
       </c>
       <c r="W2" s="16" t="str">
         <f t="shared" ref="W2" si="1">TEXT(TODAY()-100,"DD/MM/YYYY")</f>
-        <v>29/06/2024</v>
+        <v>01/07/2024</v>
       </c>
       <c r="X2" s="15" t="s">
         <v>92</v>
@@ -1384,7 +1411,7 @@
       </c>
       <c r="AH2" s="23">
         <f>W2+300</f>
-        <v>45772</v>
+        <v>45774</v>
       </c>
       <c r="AI2" s="15" t="s">
         <v>100</v>
@@ -1437,15 +1464,15 @@
       </c>
       <c r="AY2" s="16" t="str">
         <f t="shared" ref="AY2:AZ2" si="3">TEXT(TODAY()-100,"DD/MM/YYYY")</f>
-        <v>29/06/2024</v>
+        <v>01/07/2024</v>
       </c>
       <c r="AZ2" s="16" t="str">
         <f t="shared" si="3"/>
-        <v>29/06/2024</v>
+        <v>01/07/2024</v>
       </c>
       <c r="BA2" s="16" t="str">
         <f t="shared" ref="BA2" si="4">TEXT(TODAY()+200,"DD/MM/YYYY")</f>
-        <v>25/04/2025</v>
+        <v>27/04/2025</v>
       </c>
       <c r="BB2" s="25" t="s">
         <v>81</v>
@@ -1539,23 +1566,23 @@
       <c r="A3" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="31" t="s">
         <v>130</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="D3" s="12" t="s">
-        <v>80</v>
+      <c r="D3" s="32" t="s">
+        <v>131</v>
       </c>
       <c r="E3" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="F3" s="31" t="s">
-        <v>131</v>
-      </c>
-      <c r="G3" s="31" t="s">
-        <v>83</v>
+      <c r="F3" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>133</v>
       </c>
       <c r="H3" s="15">
         <v>720527700</v>
@@ -1568,7 +1595,7 @@
       </c>
       <c r="K3" s="16" t="str">
         <f>TEXT(TODAY()-100,"DD/MM/YYYY")</f>
-        <v>29/06/2024</v>
+        <v>01/07/2024</v>
       </c>
       <c r="L3" s="28" t="s">
         <v>81</v>
@@ -1597,7 +1624,7 @@
       <c r="T3" s="28" t="s">
         <v>90</v>
       </c>
-      <c r="U3" s="32" t="s">
+      <c r="U3" s="33" t="s">
         <v>91</v>
       </c>
       <c r="V3" s="29" t="s">
@@ -1605,22 +1632,22 @@
       </c>
       <c r="W3" s="16" t="str">
         <f>TEXT(TODAY()-100,"DD/MM/YYYY")</f>
-        <v>29/06/2024</v>
+        <v>01/07/2024</v>
       </c>
       <c r="X3" s="15" t="s">
         <v>92</v>
       </c>
       <c r="Y3" s="20" t="s">
-        <v>93</v>
+        <v>134</v>
       </c>
       <c r="Z3" s="18" t="s">
         <v>94</v>
       </c>
       <c r="AA3" s="13" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="AB3" s="18" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="AC3" s="13">
         <v>880</v>
@@ -1639,16 +1666,16 @@
       </c>
       <c r="AH3" s="23">
         <f>W3+300</f>
-        <v>45772</v>
+        <v>45774</v>
       </c>
       <c r="AI3" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="AJ3" s="27" t="s">
-        <v>101</v>
+      <c r="AJ3" s="34" t="s">
+        <v>137</v>
       </c>
       <c r="AK3" s="27" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="AL3" s="15" t="s">
         <v>103</v>
@@ -1692,15 +1719,15 @@
       </c>
       <c r="AY3" s="16" t="str">
         <f>TEXT(TODAY()-100,"DD/MM/YYYY")</f>
-        <v>29/06/2024</v>
+        <v>01/07/2024</v>
       </c>
       <c r="AZ3" s="16" t="str">
         <f>TEXT(TODAY()-100,"DD/MM/YYYY")</f>
-        <v>29/06/2024</v>
+        <v>01/07/2024</v>
       </c>
       <c r="BA3" s="16" t="str">
         <f>TEXT(TODAY()+200,"DD/MM/YYYY")</f>
-        <v>25/04/2025</v>
+        <v>27/04/2025</v>
       </c>
       <c r="BB3" s="25" t="s">
         <v>81</v>
@@ -1709,7 +1736,7 @@
         <v>112</v>
       </c>
       <c r="BD3" s="26">
-        <v>2330918326496</v>
+        <v>6141023089638</v>
       </c>
       <c r="BE3" s="18" t="s">
         <v>113</v>
@@ -1723,8 +1750,8 @@
       <c r="BH3" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="BI3" s="33" t="s">
-        <v>135</v>
+      <c r="BI3" s="27">
+        <v>492172</v>
       </c>
       <c r="BJ3" s="18" t="s">
         <v>113</v>
@@ -1789,12 +1816,15 @@
       <c r="CD3" s="29" t="s">
         <v>128</v>
       </c>
+    </row>
+    <row r="4" ht="15.65" customHeight="1" spans="36:36" x14ac:dyDescent="0.25">
+      <c r="AJ4" s="27"/>
     </row>
     <row r="24" ht="15.65" customHeight="1" spans="4:82" x14ac:dyDescent="0.25">
       <c r="D24" s="12"/>
       <c r="E24" s="13"/>
-      <c r="F24" s="31"/>
-      <c r="G24" s="31"/>
+      <c r="F24" s="35"/>
+      <c r="G24" s="35"/>
       <c r="H24" s="15"/>
       <c r="I24" s="15"/>
       <c r="J24" s="15"/>
@@ -1808,7 +1838,7 @@
       <c r="R24" s="15"/>
       <c r="S24" s="15"/>
       <c r="T24" s="18"/>
-      <c r="U24" s="34"/>
+      <c r="U24" s="36"/>
       <c r="V24" s="15"/>
       <c r="W24" s="16"/>
       <c r="X24" s="15"/>
@@ -1843,7 +1873,7 @@
       <c r="BA24" s="16"/>
       <c r="BB24" s="25"/>
       <c r="BC24" s="25"/>
-      <c r="BD24" s="35"/>
+      <c r="BD24" s="37"/>
       <c r="BE24" s="18"/>
       <c r="BF24" s="18"/>
       <c r="BG24" s="25"/>
@@ -1858,7 +1888,7 @@
       <c r="BP24" s="18"/>
       <c r="BQ24" s="25"/>
       <c r="BR24" s="13"/>
-      <c r="BS24" s="36"/>
+      <c r="BS24" s="38"/>
       <c r="BT24" s="25"/>
       <c r="BU24" s="25"/>
       <c r="BV24" s="13"/>
@@ -1874,8 +1904,8 @@
     <row r="25" ht="15.65" customHeight="1" spans="4:82" x14ac:dyDescent="0.25">
       <c r="D25" s="12"/>
       <c r="E25" s="13"/>
-      <c r="F25" s="31"/>
-      <c r="G25" s="31"/>
+      <c r="F25" s="35"/>
+      <c r="G25" s="35"/>
       <c r="H25" s="15"/>
       <c r="I25" s="15"/>
       <c r="J25" s="15"/>
@@ -1889,7 +1919,7 @@
       <c r="R25" s="15"/>
       <c r="S25" s="15"/>
       <c r="T25" s="18"/>
-      <c r="U25" s="34"/>
+      <c r="U25" s="36"/>
       <c r="V25" s="15"/>
       <c r="W25" s="16"/>
       <c r="X25" s="15"/>
@@ -1924,7 +1954,7 @@
       <c r="BA25" s="16"/>
       <c r="BB25" s="25"/>
       <c r="BC25" s="25"/>
-      <c r="BD25" s="35"/>
+      <c r="BD25" s="37"/>
       <c r="BE25" s="18"/>
       <c r="BF25" s="18"/>
       <c r="BG25" s="25"/>
@@ -1939,7 +1969,7 @@
       <c r="BP25" s="18"/>
       <c r="BQ25" s="25"/>
       <c r="BR25" s="13"/>
-      <c r="BS25" s="36"/>
+      <c r="BS25" s="38"/>
       <c r="BT25" s="25"/>
       <c r="BU25" s="25"/>
       <c r="BV25" s="13"/>
@@ -1955,8 +1985,8 @@
     <row r="26" ht="15.65" customHeight="1" spans="4:82" x14ac:dyDescent="0.25">
       <c r="D26" s="12"/>
       <c r="E26" s="13"/>
-      <c r="F26" s="31"/>
-      <c r="G26" s="31"/>
+      <c r="F26" s="35"/>
+      <c r="G26" s="35"/>
       <c r="H26" s="15"/>
       <c r="I26" s="15"/>
       <c r="J26" s="15"/>
@@ -1970,7 +2000,7 @@
       <c r="R26" s="15"/>
       <c r="S26" s="15"/>
       <c r="T26" s="18"/>
-      <c r="U26" s="34"/>
+      <c r="U26" s="36"/>
       <c r="V26" s="15"/>
       <c r="W26" s="16"/>
       <c r="X26" s="15"/>
@@ -2005,7 +2035,7 @@
       <c r="BA26" s="16"/>
       <c r="BB26" s="25"/>
       <c r="BC26" s="25"/>
-      <c r="BD26" s="35"/>
+      <c r="BD26" s="37"/>
       <c r="BE26" s="18"/>
       <c r="BF26" s="18"/>
       <c r="BG26" s="25"/>
@@ -2020,7 +2050,7 @@
       <c r="BP26" s="18"/>
       <c r="BQ26" s="25"/>
       <c r="BR26" s="13"/>
-      <c r="BS26" s="36"/>
+      <c r="BS26" s="38"/>
       <c r="BT26" s="25"/>
       <c r="BU26" s="25"/>
       <c r="BV26" s="13"/>
@@ -2036,8 +2066,8 @@
     <row r="27" ht="15.65" customHeight="1" spans="4:82" x14ac:dyDescent="0.25">
       <c r="D27" s="12"/>
       <c r="E27" s="13"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
+      <c r="F27" s="35"/>
+      <c r="G27" s="35"/>
       <c r="H27" s="15"/>
       <c r="I27" s="15"/>
       <c r="J27" s="15"/>
@@ -2051,7 +2081,7 @@
       <c r="R27" s="15"/>
       <c r="S27" s="15"/>
       <c r="T27" s="18"/>
-      <c r="U27" s="34"/>
+      <c r="U27" s="36"/>
       <c r="V27" s="15"/>
       <c r="W27" s="16"/>
       <c r="X27" s="15"/>
@@ -2062,7 +2092,7 @@
       <c r="AC27" s="13"/>
       <c r="AD27" s="13"/>
       <c r="AE27" s="13"/>
-      <c r="AF27" s="37"/>
+      <c r="AF27" s="39"/>
       <c r="AG27" s="13"/>
       <c r="AH27" s="23"/>
       <c r="AI27" s="15"/>
@@ -2085,7 +2115,7 @@
       <c r="BA27" s="16"/>
       <c r="BB27" s="25"/>
       <c r="BC27" s="25"/>
-      <c r="BD27" s="35"/>
+      <c r="BD27" s="37"/>
       <c r="BE27" s="18"/>
       <c r="BF27" s="18"/>
       <c r="BG27" s="25"/>
@@ -2100,7 +2130,7 @@
       <c r="BP27" s="18"/>
       <c r="BQ27" s="25"/>
       <c r="BR27" s="13"/>
-      <c r="BS27" s="36"/>
+      <c r="BS27" s="38"/>
       <c r="BT27" s="25"/>
       <c r="BU27" s="25"/>
       <c r="BV27" s="13"/>
@@ -2116,8 +2146,8 @@
     <row r="28" ht="15.65" customHeight="1" spans="4:82" x14ac:dyDescent="0.25">
       <c r="D28" s="12"/>
       <c r="E28" s="13"/>
-      <c r="F28" s="31"/>
-      <c r="G28" s="31"/>
+      <c r="F28" s="35"/>
+      <c r="G28" s="35"/>
       <c r="H28" s="15"/>
       <c r="I28" s="15"/>
       <c r="J28" s="15"/>
@@ -2131,7 +2161,7 @@
       <c r="R28" s="15"/>
       <c r="S28" s="15"/>
       <c r="T28" s="18"/>
-      <c r="U28" s="34"/>
+      <c r="U28" s="36"/>
       <c r="V28" s="15"/>
       <c r="W28" s="16"/>
       <c r="X28" s="15"/>
@@ -2142,7 +2172,7 @@
       <c r="AC28" s="13"/>
       <c r="AD28" s="13"/>
       <c r="AE28" s="13"/>
-      <c r="AF28" s="37"/>
+      <c r="AF28" s="39"/>
       <c r="AG28" s="13"/>
       <c r="AH28" s="23"/>
       <c r="AI28" s="15"/>
@@ -2166,7 +2196,7 @@
       <c r="BA28" s="16"/>
       <c r="BB28" s="25"/>
       <c r="BC28" s="25"/>
-      <c r="BD28" s="35"/>
+      <c r="BD28" s="37"/>
       <c r="BE28" s="18"/>
       <c r="BF28" s="18"/>
       <c r="BG28" s="25"/>
@@ -2181,7 +2211,7 @@
       <c r="BP28" s="18"/>
       <c r="BQ28" s="25"/>
       <c r="BR28" s="13"/>
-      <c r="BS28" s="36"/>
+      <c r="BS28" s="38"/>
       <c r="BT28" s="25"/>
       <c r="BU28" s="25"/>
       <c r="BV28" s="13"/>
@@ -2197,8 +2227,8 @@
     <row r="29" ht="15.65" customHeight="1" spans="4:82" x14ac:dyDescent="0.25">
       <c r="D29" s="12"/>
       <c r="E29" s="13"/>
-      <c r="F29" s="31"/>
-      <c r="G29" s="31"/>
+      <c r="F29" s="35"/>
+      <c r="G29" s="35"/>
       <c r="H29" s="15"/>
       <c r="I29" s="15"/>
       <c r="J29" s="15"/>
@@ -2212,7 +2242,7 @@
       <c r="R29" s="15"/>
       <c r="S29" s="15"/>
       <c r="T29" s="18"/>
-      <c r="U29" s="34"/>
+      <c r="U29" s="36"/>
       <c r="V29" s="15"/>
       <c r="W29" s="16"/>
       <c r="X29" s="15"/>
@@ -2247,7 +2277,7 @@
       <c r="BA29" s="16"/>
       <c r="BB29" s="25"/>
       <c r="BC29" s="25"/>
-      <c r="BD29" s="35"/>
+      <c r="BD29" s="37"/>
       <c r="BE29" s="18"/>
       <c r="BF29" s="18"/>
       <c r="BG29" s="25"/>
@@ -2262,7 +2292,7 @@
       <c r="BP29" s="18"/>
       <c r="BQ29" s="25"/>
       <c r="BR29" s="13"/>
-      <c r="BS29" s="36"/>
+      <c r="BS29" s="38"/>
       <c r="BT29" s="25"/>
       <c r="BU29" s="25"/>
       <c r="BV29" s="13"/>
@@ -2278,8 +2308,8 @@
     <row r="30" ht="15.65" customHeight="1" spans="4:82" x14ac:dyDescent="0.25">
       <c r="D30" s="12"/>
       <c r="E30" s="13"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="31"/>
+      <c r="F30" s="35"/>
+      <c r="G30" s="35"/>
       <c r="H30" s="15"/>
       <c r="I30" s="15"/>
       <c r="J30" s="15"/>
@@ -2293,7 +2323,7 @@
       <c r="R30" s="15"/>
       <c r="S30" s="15"/>
       <c r="T30" s="18"/>
-      <c r="U30" s="34"/>
+      <c r="U30" s="36"/>
       <c r="V30" s="15"/>
       <c r="W30" s="16"/>
       <c r="X30" s="15"/>
@@ -2328,7 +2358,7 @@
       <c r="BA30" s="16"/>
       <c r="BB30" s="25"/>
       <c r="BC30" s="25"/>
-      <c r="BD30" s="35"/>
+      <c r="BD30" s="37"/>
       <c r="BE30" s="18"/>
       <c r="BF30" s="18"/>
       <c r="BG30" s="25"/>
@@ -2343,7 +2373,7 @@
       <c r="BP30" s="18"/>
       <c r="BQ30" s="25"/>
       <c r="BR30" s="13"/>
-      <c r="BS30" s="36"/>
+      <c r="BS30" s="38"/>
       <c r="BT30" s="25"/>
       <c r="BU30" s="25"/>
       <c r="BV30" s="13"/>
@@ -2359,8 +2389,8 @@
     <row r="32" ht="15.65" customHeight="1" spans="4:82" x14ac:dyDescent="0.25">
       <c r="D32" s="12"/>
       <c r="E32" s="13"/>
-      <c r="F32" s="31"/>
-      <c r="G32" s="31"/>
+      <c r="F32" s="35"/>
+      <c r="G32" s="35"/>
       <c r="H32" s="15"/>
       <c r="I32" s="15"/>
       <c r="J32" s="15"/>
@@ -2374,7 +2404,7 @@
       <c r="R32" s="15"/>
       <c r="S32" s="15"/>
       <c r="T32" s="18"/>
-      <c r="U32" s="34"/>
+      <c r="U32" s="36"/>
       <c r="V32" s="15"/>
       <c r="W32" s="16"/>
       <c r="X32" s="15"/>
@@ -2409,7 +2439,7 @@
       <c r="BA32" s="16"/>
       <c r="BB32" s="25"/>
       <c r="BC32" s="25"/>
-      <c r="BD32" s="35"/>
+      <c r="BD32" s="37"/>
       <c r="BE32" s="18"/>
       <c r="BF32" s="18"/>
       <c r="BG32" s="25"/>
@@ -2424,7 +2454,7 @@
       <c r="BP32" s="18"/>
       <c r="BQ32" s="25"/>
       <c r="BR32" s="13"/>
-      <c r="BS32" s="36"/>
+      <c r="BS32" s="38"/>
       <c r="BT32" s="25"/>
       <c r="BU32" s="25"/>
       <c r="BV32" s="13"/>

</xml_diff>

<commit_message>
Latest code for Romania
</commit_message>
<xml_diff>
--- a/Data/testDataRomania.xlsx
+++ b/Data/testDataRomania.xlsx
@@ -1,20 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{62C1033C-6C4C-4C47-8D90-446003281065}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Sheet2" state="visible" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1043" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1046" uniqueCount="172">
   <si>
     <t>TestCaseIDs</t>
   </si>
@@ -250,7 +265,7 @@
     <t>Test1</t>
   </si>
   <si>
-    <t>Test failed for 'Ansley Mueller-Stoltenberg' Employee:{undefined}Error: page.waitForTimeout: Target page, context or browser has been closed</t>
+    <t>Test failed for 'Cara Crooks' Employee:{undefined}TypeError: Cannot read properties of undefined (reading 'split')</t>
   </si>
   <si>
     <t>Failed</t>
@@ -262,10 +277,10 @@
     <t>Romania</t>
   </si>
   <si>
-    <t>Ansley</t>
-  </si>
-  <si>
-    <t>Mueller-Stoltenberg</t>
+    <t>Cara</t>
+  </si>
+  <si>
+    <t>Crooks</t>
   </si>
   <si>
     <t>Mobile</t>
@@ -406,6 +421,18 @@
     <t>Test2</t>
   </si>
   <si>
+    <t xml:space="preserve">Test failed for 'Kenna Balistreri' Employee:{10651067}TimeoutError: locator.click: Timeout 30000ms exceeded.
+Call log:
+  [2m- waiting for locator('text=Onboarding Guide: Retail Assistant_NEW - Kenna Balistreri')[22m
+</t>
+  </si>
+  <si>
+    <t>Kenna</t>
+  </si>
+  <si>
+    <t>Balistreri</t>
+  </si>
+  <si>
     <t>Fixed Term (Fixed Term)</t>
   </si>
   <si>
@@ -427,7 +454,7 @@
     <t>Store Manager_NEW</t>
   </si>
   <si>
-    <t xml:space="preserve">92 Retail Management </t>
+    <t>92 Retail Management </t>
   </si>
   <si>
     <t>251 Management Retail</t>
@@ -527,51 +554,51 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <color rgb="FFFF0000"/>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <family val="2"/>
-      <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <color theme="4"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <u/>
+      <sz val="11"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
     <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="4">
@@ -583,7 +610,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.5999938962981048"/>
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -608,8 +635,12 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -619,17 +650,27 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin"/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -1052,14 +1093,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CD32"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="BI5" sqref="BI5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.65" outlineLevelRow="1" outlineLevelCol="0" x14ac:dyDescent="0.35" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="15.65" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.81640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="11.81640625" style="1" customWidth="1"/>
@@ -1145,7 +1186,7 @@
     <col min="83" max="83" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.5" customHeight="1" spans="1:82" s="3" customFormat="1" x14ac:dyDescent="0.25" outlineLevel="1" collapsed="1">
+    <row r="1" spans="1:82" s="3" customFormat="1" ht="14.5" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1393,7 +1434,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" ht="15.65" customHeight="1" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:82" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>77</v>
       </c>
@@ -1425,7 +1466,7 @@
         <v>85</v>
       </c>
       <c r="K2" s="15" t="str">
-        <f t="shared" ref="K2:K16" si="0">TEXT(TODAY()-100,"DD/MM/YYYY")</f>
+        <f t="shared" ref="K2:K16" ca="1" si="0">TEXT(TODAY()-100,"DD/MM/YYYY")</f>
         <v>07/07/2024</v>
       </c>
       <c r="L2" s="12" t="s">
@@ -1462,7 +1503,7 @@
         <v>85</v>
       </c>
       <c r="W2" s="15" t="str">
-        <f t="shared" ref="W2:W16" si="1">TEXT(TODAY()-100,"DD/MM/YYYY")</f>
+        <f t="shared" ref="W2:W16" ca="1" si="1">TEXT(TODAY()-100,"DD/MM/YYYY")</f>
         <v>07/07/2024</v>
       </c>
       <c r="X2" s="14" t="s">
@@ -1531,9 +1572,9 @@
       <c r="AS2" s="14">
         <v>1</v>
       </c>
-      <c r="AT2" s="28">
-        <f t="shared" ref="AT2:AT16" si="2">TEXT(TODAY()-100,"DD/MM/YYYY")</f>
-        <v>NaN</v>
+      <c r="AT2" s="28" t="str">
+        <f t="shared" ref="AT2:AT16" ca="1" si="2">TEXT(TODAY()-100,"DD/MM/YYYY")</f>
+        <v>07/07/2024</v>
       </c>
       <c r="AU2" s="12" t="s">
         <v>100</v>
@@ -1548,11 +1589,11 @@
         <v>111</v>
       </c>
       <c r="AY2" s="15" t="str">
-        <f t="shared" ref="AY2:AZ16" si="3">TEXT(TODAY()-100,"DD/MM/YYYY")</f>
+        <f t="shared" ref="AY2:AZ16" ca="1" si="3">TEXT(TODAY()-100,"DD/MM/YYYY")</f>
         <v>07/07/2024</v>
       </c>
       <c r="AZ2" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ca="1" si="3"/>
         <v>07/07/2024</v>
       </c>
       <c r="BA2" s="24" t="s">
@@ -1565,7 +1606,7 @@
         <v>112</v>
       </c>
       <c r="BD2" s="30">
-        <v>2920706247609</v>
+        <v>2290811241729</v>
       </c>
       <c r="BE2" s="17" t="s">
         <v>113</v>
@@ -1580,7 +1621,7 @@
         <v>115</v>
       </c>
       <c r="BI2" s="31">
-        <v>354399</v>
+        <v>364399</v>
       </c>
       <c r="BJ2" s="17" t="s">
         <v>113</v>
@@ -1646,11 +1687,13 @@
         <v>128</v>
       </c>
     </row>
-    <row r="3" ht="15.65" customHeight="1" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:82" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B3" s="9"/>
+      <c r="B3" s="9" t="s">
+        <v>130</v>
+      </c>
       <c r="C3" s="10" t="s">
         <v>79</v>
       </c>
@@ -1660,8 +1703,12 @@
       <c r="E3" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
+      <c r="F3" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>132</v>
+      </c>
       <c r="H3" s="14">
         <v>720527700</v>
       </c>
@@ -1672,7 +1719,7 @@
         <v>85</v>
       </c>
       <c r="K3" s="15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>07/07/2024</v>
       </c>
       <c r="L3" s="32" t="s">
@@ -1709,7 +1756,7 @@
         <v>85</v>
       </c>
       <c r="W3" s="15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ca="1" si="1"/>
         <v>07/07/2024</v>
       </c>
       <c r="X3" s="14" t="s">
@@ -1719,13 +1766,13 @@
         <v>93</v>
       </c>
       <c r="Z3" s="19" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="AA3" s="20" t="s">
         <v>95</v>
       </c>
       <c r="AB3" s="19" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="AC3" s="21">
         <v>880</v>
@@ -1743,7 +1790,7 @@
         <v>99</v>
       </c>
       <c r="AH3" s="35" t="str">
-        <f t="shared" ref="AH3:AH5" si="4">TEXT(TODAY()+200,"DD/MM/YYYY")</f>
+        <f t="shared" ref="AH3:AH5" ca="1" si="4">TEXT(TODAY()+200,"DD/MM/YYYY")</f>
         <v>03/05/2025</v>
       </c>
       <c r="AI3" s="14" t="s">
@@ -1753,7 +1800,7 @@
         <v>102</v>
       </c>
       <c r="AK3" s="25" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="AL3" s="14" t="s">
         <v>104</v>
@@ -1779,9 +1826,9 @@
       <c r="AS3" s="14">
         <v>2</v>
       </c>
-      <c r="AT3" s="28">
-        <f t="shared" si="2"/>
-        <v>NaN</v>
+      <c r="AT3" s="28" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>07/07/2024</v>
       </c>
       <c r="AU3" s="12" t="s">
         <v>100</v>
@@ -1796,15 +1843,15 @@
         <v>111</v>
       </c>
       <c r="AY3" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ca="1" si="3"/>
         <v>07/07/2024</v>
       </c>
       <c r="AZ3" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ca="1" si="3"/>
         <v>07/07/2024</v>
       </c>
       <c r="BA3" s="35" t="str">
-        <f>TEXT(TODAY()+200,"DD/MM/YYYY")</f>
+        <f ca="1">TEXT(TODAY()+200,"DD/MM/YYYY")</f>
         <v>03/05/2025</v>
       </c>
       <c r="BB3" s="29" t="s">
@@ -1814,7 +1861,7 @@
         <v>112</v>
       </c>
       <c r="BD3" s="30">
-        <v>6130528367644</v>
+        <v>2370809180007</v>
       </c>
       <c r="BE3" s="17" t="s">
         <v>113</v>
@@ -1829,7 +1876,7 @@
         <v>115</v>
       </c>
       <c r="BI3" s="31">
-        <v>264400</v>
+        <v>364400</v>
       </c>
       <c r="BJ3" s="17" t="s">
         <v>113</v>
@@ -1895,16 +1942,16 @@
         <v>128</v>
       </c>
     </row>
-    <row r="4" ht="15.65" customHeight="1" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:82" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="10" t="s">
         <v>79</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>81</v>
@@ -1921,7 +1968,7 @@
         <v>85</v>
       </c>
       <c r="K4" s="15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>07/07/2024</v>
       </c>
       <c r="L4" s="12" t="s">
@@ -1958,20 +2005,20 @@
         <v>85</v>
       </c>
       <c r="W4" s="15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ca="1" si="1"/>
         <v>07/07/2024</v>
       </c>
       <c r="X4" s="14" t="s">
         <v>92</v>
       </c>
       <c r="Y4" s="17" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="Z4" s="19" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="AA4" s="36" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="AB4" s="19" t="s">
         <v>96</v>
@@ -1992,17 +2039,17 @@
         <v>99</v>
       </c>
       <c r="AH4" s="35" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ca="1" si="4"/>
         <v>03/05/2025</v>
       </c>
       <c r="AI4" s="14" t="s">
         <v>101</v>
       </c>
       <c r="AJ4" s="37" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="AK4" s="38" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="AL4" s="14" t="s">
         <v>104</v>
@@ -2028,9 +2075,9 @@
       <c r="AS4" s="14">
         <v>3</v>
       </c>
-      <c r="AT4" s="28">
-        <f t="shared" si="2"/>
-        <v>NaN</v>
+      <c r="AT4" s="28" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>07/07/2024</v>
       </c>
       <c r="AU4" s="12" t="s">
         <v>100</v>
@@ -2045,15 +2092,15 @@
         <v>111</v>
       </c>
       <c r="AY4" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ca="1" si="3"/>
         <v>07/07/2024</v>
       </c>
       <c r="AZ4" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ca="1" si="3"/>
         <v>07/07/2024</v>
       </c>
       <c r="BA4" s="35" t="str">
-        <f t="shared" ref="BA4:BA5" si="5">TEXT(TODAY()+200,"DD/MM/YYYY")</f>
+        <f t="shared" ref="BA4:BA5" ca="1" si="5">TEXT(TODAY()+200,"DD/MM/YYYY")</f>
         <v>03/05/2025</v>
       </c>
       <c r="BB4" s="29" t="s">
@@ -2144,16 +2191,16 @@
         <v>128</v>
       </c>
     </row>
-    <row r="5" ht="15.65" customHeight="1" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:82" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="B5" s="9"/>
       <c r="C5" s="10" t="s">
         <v>79</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>81</v>
@@ -2170,7 +2217,7 @@
         <v>85</v>
       </c>
       <c r="K5" s="15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>07/07/2024</v>
       </c>
       <c r="L5" s="32" t="s">
@@ -2207,23 +2254,23 @@
         <v>85</v>
       </c>
       <c r="W5" s="15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ca="1" si="1"/>
         <v>07/07/2024</v>
       </c>
       <c r="X5" s="14" t="s">
         <v>92</v>
       </c>
       <c r="Y5" s="17" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="Z5" s="19" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="AA5" s="19" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="AB5" s="20" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="AC5" s="21">
         <v>880</v>
@@ -2241,17 +2288,17 @@
         <v>99</v>
       </c>
       <c r="AH5" s="35" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ca="1" si="4"/>
         <v>03/05/2025</v>
       </c>
       <c r="AI5" s="14" t="s">
         <v>101</v>
       </c>
       <c r="AJ5" s="37" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="AK5" s="38" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="AL5" s="14" t="s">
         <v>104</v>
@@ -2277,9 +2324,9 @@
       <c r="AS5" s="14">
         <v>1</v>
       </c>
-      <c r="AT5" s="28">
-        <f t="shared" si="2"/>
-        <v>NaN</v>
+      <c r="AT5" s="28" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>07/07/2024</v>
       </c>
       <c r="AU5" s="12" t="s">
         <v>100</v>
@@ -2294,15 +2341,15 @@
         <v>111</v>
       </c>
       <c r="AY5" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ca="1" si="3"/>
         <v>07/07/2024</v>
       </c>
       <c r="AZ5" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ca="1" si="3"/>
         <v>07/07/2024</v>
       </c>
       <c r="BA5" s="35" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>03/05/2025</v>
       </c>
       <c r="BB5" s="29" t="s">
@@ -2393,14 +2440,14 @@
         <v>128</v>
       </c>
     </row>
-    <row r="6" ht="15.65" customHeight="1" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:82" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B6" s="9"/>
       <c r="C6" s="10"/>
       <c r="D6" s="11" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="E6" s="12" t="s">
         <v>81</v>
@@ -2417,7 +2464,7 @@
         <v>85</v>
       </c>
       <c r="K6" s="15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>07/07/2024</v>
       </c>
       <c r="L6" s="12" t="s">
@@ -2454,20 +2501,20 @@
         <v>85</v>
       </c>
       <c r="W6" s="15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ca="1" si="1"/>
         <v>07/07/2024</v>
       </c>
       <c r="X6" s="14" t="s">
         <v>92</v>
       </c>
       <c r="Y6" s="17" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="Z6" s="19" t="s">
         <v>94</v>
       </c>
       <c r="AA6" s="19" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="AB6" s="20" t="s">
         <v>96</v>
@@ -2494,10 +2541,10 @@
         <v>101</v>
       </c>
       <c r="AJ6" s="37" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="AK6" s="38" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="AL6" s="14" t="s">
         <v>104</v>
@@ -2523,9 +2570,9 @@
       <c r="AS6" s="14">
         <v>2</v>
       </c>
-      <c r="AT6" s="28">
-        <f t="shared" si="2"/>
-        <v>NaN</v>
+      <c r="AT6" s="28" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>07/07/2024</v>
       </c>
       <c r="AU6" s="12" t="s">
         <v>100</v>
@@ -2540,11 +2587,11 @@
         <v>111</v>
       </c>
       <c r="AY6" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ca="1" si="3"/>
         <v>07/07/2024</v>
       </c>
       <c r="AZ6" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ca="1" si="3"/>
         <v>07/07/2024</v>
       </c>
       <c r="BA6" s="24" t="str">
@@ -2639,14 +2686,14 @@
         <v>128</v>
       </c>
     </row>
-    <row r="7" ht="15.65" customHeight="1" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:82" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B7" s="9"/>
       <c r="C7" s="10"/>
       <c r="D7" s="11" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>81</v>
@@ -2663,7 +2710,7 @@
         <v>85</v>
       </c>
       <c r="K7" s="15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>07/07/2024</v>
       </c>
       <c r="L7" s="32" t="s">
@@ -2700,23 +2747,23 @@
         <v>85</v>
       </c>
       <c r="W7" s="15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ca="1" si="1"/>
         <v>07/07/2024</v>
       </c>
       <c r="X7" s="14" t="s">
         <v>92</v>
       </c>
       <c r="Y7" s="17" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="Z7" s="19" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="AA7" s="19" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="AB7" s="36" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="AC7" s="21">
         <v>880</v>
@@ -2734,17 +2781,17 @@
         <v>99</v>
       </c>
       <c r="AH7" s="35" t="str">
-        <f>TEXT(TODAY()+200,"DD/MM/YYYY")</f>
+        <f ca="1">TEXT(TODAY()+200,"DD/MM/YYYY")</f>
         <v>03/05/2025</v>
       </c>
       <c r="AI7" s="14" t="s">
         <v>101</v>
       </c>
       <c r="AJ7" s="37" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="AK7" s="38" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="AL7" s="14" t="s">
         <v>104</v>
@@ -2770,9 +2817,9 @@
       <c r="AS7" s="14">
         <v>3</v>
       </c>
-      <c r="AT7" s="28">
-        <f t="shared" si="2"/>
-        <v>NaN</v>
+      <c r="AT7" s="28" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>07/07/2024</v>
       </c>
       <c r="AU7" s="12" t="s">
         <v>100</v>
@@ -2787,15 +2834,15 @@
         <v>111</v>
       </c>
       <c r="AY7" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ca="1" si="3"/>
         <v>07/07/2024</v>
       </c>
       <c r="AZ7" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ca="1" si="3"/>
         <v>07/07/2024</v>
       </c>
       <c r="BA7" s="35" t="str">
-        <f>TEXT(TODAY()+200,"DD/MM/YYYY")</f>
+        <f ca="1">TEXT(TODAY()+200,"DD/MM/YYYY")</f>
         <v>03/05/2025</v>
       </c>
       <c r="BB7" s="29" t="s">
@@ -2886,14 +2933,14 @@
         <v>128</v>
       </c>
     </row>
-    <row r="8" ht="15.65" customHeight="1" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:82" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="10"/>
       <c r="D8" s="11" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="E8" s="12" t="s">
         <v>81</v>
@@ -2910,7 +2957,7 @@
         <v>85</v>
       </c>
       <c r="K8" s="15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>07/07/2024</v>
       </c>
       <c r="L8" s="12" t="s">
@@ -2947,20 +2994,20 @@
         <v>85</v>
       </c>
       <c r="W8" s="15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ca="1" si="1"/>
         <v>07/07/2024</v>
       </c>
       <c r="X8" s="14" t="s">
         <v>92</v>
       </c>
       <c r="Y8" s="17" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="Z8" s="19" t="s">
         <v>94</v>
       </c>
       <c r="AA8" s="19" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="AB8" s="36" t="s">
         <v>96</v>
@@ -2987,10 +3034,10 @@
         <v>101</v>
       </c>
       <c r="AJ8" s="37" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="AK8" s="38" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="AL8" s="14" t="s">
         <v>104</v>
@@ -3016,9 +3063,9 @@
       <c r="AS8" s="14">
         <v>1</v>
       </c>
-      <c r="AT8" s="28">
-        <f t="shared" si="2"/>
-        <v>NaN</v>
+      <c r="AT8" s="28" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>07/07/2024</v>
       </c>
       <c r="AU8" s="12" t="s">
         <v>100</v>
@@ -3033,11 +3080,11 @@
         <v>111</v>
       </c>
       <c r="AY8" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ca="1" si="3"/>
         <v>07/07/2024</v>
       </c>
       <c r="AZ8" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ca="1" si="3"/>
         <v>07/07/2024</v>
       </c>
       <c r="BA8" s="24" t="str">
@@ -3132,14 +3179,14 @@
         <v>128</v>
       </c>
     </row>
-    <row r="9" ht="15.65" customHeight="1" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:82" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="10"/>
       <c r="D9" s="11" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="E9" s="12" t="s">
         <v>81</v>
@@ -3156,7 +3203,7 @@
         <v>85</v>
       </c>
       <c r="K9" s="15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>07/07/2024</v>
       </c>
       <c r="L9" s="32" t="s">
@@ -3193,23 +3240,23 @@
         <v>85</v>
       </c>
       <c r="W9" s="15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ca="1" si="1"/>
         <v>07/07/2024</v>
       </c>
       <c r="X9" s="14" t="s">
         <v>92</v>
       </c>
       <c r="Y9" s="17" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="Z9" s="19" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="AA9" s="19" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="AB9" s="20" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="AC9" s="21">
         <v>880</v>
@@ -3227,17 +3274,17 @@
         <v>99</v>
       </c>
       <c r="AH9" s="35" t="str">
-        <f>TEXT(TODAY()+200,"DD/MM/YYYY")</f>
+        <f ca="1">TEXT(TODAY()+200,"DD/MM/YYYY")</f>
         <v>03/05/2025</v>
       </c>
       <c r="AI9" s="14" t="s">
         <v>101</v>
       </c>
       <c r="AJ9" s="37" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="AK9" s="38" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="AL9" s="14" t="s">
         <v>104</v>
@@ -3263,9 +3310,9 @@
       <c r="AS9" s="14">
         <v>2</v>
       </c>
-      <c r="AT9" s="28">
-        <f t="shared" si="2"/>
-        <v>NaN</v>
+      <c r="AT9" s="28" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>07/07/2024</v>
       </c>
       <c r="AU9" s="12" t="s">
         <v>100</v>
@@ -3280,15 +3327,15 @@
         <v>111</v>
       </c>
       <c r="AY9" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ca="1" si="3"/>
         <v>07/07/2024</v>
       </c>
       <c r="AZ9" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ca="1" si="3"/>
         <v>07/07/2024</v>
       </c>
       <c r="BA9" s="35" t="str">
-        <f>TEXT(TODAY()+200,"DD/MM/YYYY")</f>
+        <f ca="1">TEXT(TODAY()+200,"DD/MM/YYYY")</f>
         <v>03/05/2025</v>
       </c>
       <c r="BB9" s="29" t="s">
@@ -3379,9 +3426,9 @@
         <v>128</v>
       </c>
     </row>
-    <row r="10" ht="15.65" customHeight="1" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:82" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="11" t="s">
@@ -3402,7 +3449,7 @@
         <v>85</v>
       </c>
       <c r="K10" s="15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>07/07/2024</v>
       </c>
       <c r="L10" s="12" t="s">
@@ -3439,7 +3486,7 @@
         <v>85</v>
       </c>
       <c r="W10" s="15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ca="1" si="1"/>
         <v>07/07/2024</v>
       </c>
       <c r="X10" s="14" t="s">
@@ -3452,7 +3499,7 @@
         <v>94</v>
       </c>
       <c r="AA10" s="19" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="AB10" s="20" t="s">
         <v>96</v>
@@ -3482,7 +3529,7 @@
         <v>102</v>
       </c>
       <c r="AK10" s="25" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="AL10" s="14" t="s">
         <v>104</v>
@@ -3503,14 +3550,14 @@
         <v>109</v>
       </c>
       <c r="AR10" s="14" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="AS10" s="14">
         <v>3</v>
       </c>
-      <c r="AT10" s="28">
-        <f t="shared" si="2"/>
-        <v>NaN</v>
+      <c r="AT10" s="28" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>07/07/2024</v>
       </c>
       <c r="AU10" s="12" t="s">
         <v>100</v>
@@ -3525,11 +3572,11 @@
         <v>111</v>
       </c>
       <c r="AY10" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ca="1" si="3"/>
         <v>07/07/2024</v>
       </c>
       <c r="AZ10" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ca="1" si="3"/>
         <v>07/07/2024</v>
       </c>
       <c r="BA10" s="40" t="str">
@@ -3624,9 +3671,9 @@
         <v>128</v>
       </c>
     </row>
-    <row r="11" ht="15.65" customHeight="1" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:82" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="11" t="s">
@@ -3647,7 +3694,7 @@
         <v>85</v>
       </c>
       <c r="K11" s="15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>07/07/2024</v>
       </c>
       <c r="L11" s="32" t="s">
@@ -3684,7 +3731,7 @@
         <v>85</v>
       </c>
       <c r="W11" s="15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ca="1" si="1"/>
         <v>07/07/2024</v>
       </c>
       <c r="X11" s="14" t="s">
@@ -3694,13 +3741,13 @@
         <v>93</v>
       </c>
       <c r="Z11" s="19" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="AA11" s="19" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="AB11" s="20" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="AC11" s="21">
         <v>880</v>
@@ -3718,7 +3765,7 @@
         <v>99</v>
       </c>
       <c r="AH11" s="35" t="str">
-        <f>TEXT(TODAY()+200,"DD/MM/YYYY")</f>
+        <f ca="1">TEXT(TODAY()+200,"DD/MM/YYYY")</f>
         <v>03/05/2025</v>
       </c>
       <c r="AI11" s="14" t="s">
@@ -3728,7 +3775,7 @@
         <v>102</v>
       </c>
       <c r="AK11" s="25" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="AL11" s="14" t="s">
         <v>104</v>
@@ -3749,14 +3796,14 @@
         <v>109</v>
       </c>
       <c r="AR11" s="14" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="AS11" s="14">
         <v>1</v>
       </c>
-      <c r="AT11" s="28">
-        <f t="shared" si="2"/>
-        <v>NaN</v>
+      <c r="AT11" s="28" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>07/07/2024</v>
       </c>
       <c r="AU11" s="12" t="s">
         <v>100</v>
@@ -3771,15 +3818,15 @@
         <v>111</v>
       </c>
       <c r="AY11" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ca="1" si="3"/>
         <v>07/07/2024</v>
       </c>
       <c r="AZ11" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ca="1" si="3"/>
         <v>07/07/2024</v>
       </c>
       <c r="BA11" s="35" t="str">
-        <f>TEXT(TODAY()+200,"DD/MM/YYYY")</f>
+        <f ca="1">TEXT(TODAY()+200,"DD/MM/YYYY")</f>
         <v>03/05/2025</v>
       </c>
       <c r="BB11" s="29" t="s">
@@ -3870,9 +3917,9 @@
         <v>128</v>
       </c>
     </row>
-    <row r="12" ht="15.65" customHeight="1" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:82" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="11" t="s">
@@ -3893,7 +3940,7 @@
         <v>85</v>
       </c>
       <c r="K12" s="15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>07/07/2024</v>
       </c>
       <c r="L12" s="12" t="s">
@@ -3930,7 +3977,7 @@
         <v>85</v>
       </c>
       <c r="W12" s="15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ca="1" si="1"/>
         <v>07/07/2024</v>
       </c>
       <c r="X12" s="14" t="s">
@@ -3943,7 +3990,7 @@
         <v>94</v>
       </c>
       <c r="AA12" s="19" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="AB12" s="20" t="s">
         <v>96</v>
@@ -3973,7 +4020,7 @@
         <v>102</v>
       </c>
       <c r="AK12" s="25" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="AL12" s="14" t="s">
         <v>104</v>
@@ -3994,14 +4041,14 @@
         <v>106</v>
       </c>
       <c r="AR12" s="14" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="AS12" s="14">
         <v>2</v>
       </c>
-      <c r="AT12" s="28">
-        <f t="shared" si="2"/>
-        <v>NaN</v>
+      <c r="AT12" s="28" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>07/07/2024</v>
       </c>
       <c r="AU12" s="12" t="s">
         <v>100</v>
@@ -4016,11 +4063,11 @@
         <v>111</v>
       </c>
       <c r="AY12" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ca="1" si="3"/>
         <v>07/07/2024</v>
       </c>
       <c r="AZ12" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ca="1" si="3"/>
         <v>07/07/2024</v>
       </c>
       <c r="BA12" s="40" t="str">
@@ -4115,9 +4162,9 @@
         <v>128</v>
       </c>
     </row>
-    <row r="13" ht="15.65" customHeight="1" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:82" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="C13" s="10"/>
       <c r="D13" s="11" t="s">
@@ -4138,7 +4185,7 @@
         <v>85</v>
       </c>
       <c r="K13" s="15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>07/07/2024</v>
       </c>
       <c r="L13" s="32" t="s">
@@ -4175,7 +4222,7 @@
         <v>85</v>
       </c>
       <c r="W13" s="15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ca="1" si="1"/>
         <v>07/07/2024</v>
       </c>
       <c r="X13" s="14" t="s">
@@ -4185,13 +4232,13 @@
         <v>93</v>
       </c>
       <c r="Z13" s="19" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="AA13" s="19" t="s">
         <v>95</v>
       </c>
       <c r="AB13" s="20" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="AC13" s="21">
         <v>880</v>
@@ -4209,7 +4256,7 @@
         <v>99</v>
       </c>
       <c r="AH13" s="35" t="str">
-        <f>TEXT(TODAY()+200,"DD/MM/YYYY")</f>
+        <f ca="1">TEXT(TODAY()+200,"DD/MM/YYYY")</f>
         <v>03/05/2025</v>
       </c>
       <c r="AI13" s="14" t="s">
@@ -4219,7 +4266,7 @@
         <v>102</v>
       </c>
       <c r="AK13" s="25" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="AL13" s="14" t="s">
         <v>104</v>
@@ -4240,14 +4287,14 @@
         <v>109</v>
       </c>
       <c r="AR13" s="14" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="AS13" s="14">
         <v>3</v>
       </c>
-      <c r="AT13" s="28">
-        <f t="shared" si="2"/>
-        <v>NaN</v>
+      <c r="AT13" s="28" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>07/07/2024</v>
       </c>
       <c r="AU13" s="12" t="s">
         <v>100</v>
@@ -4262,15 +4309,15 @@
         <v>111</v>
       </c>
       <c r="AY13" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ca="1" si="3"/>
         <v>07/07/2024</v>
       </c>
       <c r="AZ13" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ca="1" si="3"/>
         <v>07/07/2024</v>
       </c>
       <c r="BA13" s="35" t="str">
-        <f>TEXT(TODAY()+200,"DD/MM/YYYY")</f>
+        <f ca="1">TEXT(TODAY()+200,"DD/MM/YYYY")</f>
         <v>03/05/2025</v>
       </c>
       <c r="BB13" s="29" t="s">
@@ -4361,9 +4408,9 @@
         <v>128</v>
       </c>
     </row>
-    <row r="14" ht="15.65" customHeight="1" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:82" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="B14" s="41"/>
       <c r="C14" s="10"/>
@@ -4385,7 +4432,7 @@
         <v>85</v>
       </c>
       <c r="K14" s="15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>07/07/2024</v>
       </c>
       <c r="L14" s="12" t="s">
@@ -4422,7 +4469,7 @@
         <v>85</v>
       </c>
       <c r="W14" s="15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ca="1" si="1"/>
         <v>07/07/2024</v>
       </c>
       <c r="X14" s="14" t="s">
@@ -4438,7 +4485,7 @@
         <v>95</v>
       </c>
       <c r="AB14" s="20" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="AC14" s="21">
         <v>880</v>
@@ -4465,7 +4512,7 @@
         <v>102</v>
       </c>
       <c r="AK14" s="25" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="AL14" s="14" t="s">
         <v>104</v>
@@ -4486,14 +4533,14 @@
         <v>106</v>
       </c>
       <c r="AR14" s="14" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="AS14" s="14">
         <v>1</v>
       </c>
-      <c r="AT14" s="28">
-        <f t="shared" si="2"/>
-        <v>NaN</v>
+      <c r="AT14" s="28" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>07/07/2024</v>
       </c>
       <c r="AU14" s="12" t="s">
         <v>100</v>
@@ -4508,11 +4555,11 @@
         <v>111</v>
       </c>
       <c r="AY14" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ca="1" si="3"/>
         <v>07/07/2024</v>
       </c>
       <c r="AZ14" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ca="1" si="3"/>
         <v>07/07/2024</v>
       </c>
       <c r="BA14" s="40" t="str">
@@ -4607,13 +4654,13 @@
         <v>128</v>
       </c>
     </row>
-    <row r="15" ht="15.65" customHeight="1" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:82" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="C15" s="10"/>
       <c r="D15" s="11" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="E15" s="12" t="s">
         <v>81</v>
@@ -4630,7 +4677,7 @@
         <v>85</v>
       </c>
       <c r="K15" s="15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>07/07/2024</v>
       </c>
       <c r="L15" s="32" t="s">
@@ -4667,23 +4714,23 @@
         <v>85</v>
       </c>
       <c r="W15" s="15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ca="1" si="1"/>
         <v>07/07/2024</v>
       </c>
       <c r="X15" s="14" t="s">
         <v>92</v>
       </c>
       <c r="Y15" s="17" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="Z15" s="19" t="s">
         <v>94</v>
       </c>
       <c r="AA15" s="19" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="AB15" s="20" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="AC15" s="21">
         <v>880</v>
@@ -4707,10 +4754,10 @@
         <v>101</v>
       </c>
       <c r="AJ15" s="37" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="AK15" s="38" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="AL15" s="14" t="s">
         <v>104</v>
@@ -4731,14 +4778,14 @@
         <v>109</v>
       </c>
       <c r="AR15" s="14" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="AS15" s="14">
         <v>2</v>
       </c>
-      <c r="AT15" s="28">
-        <f t="shared" si="2"/>
-        <v>NaN</v>
+      <c r="AT15" s="28" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>07/07/2024</v>
       </c>
       <c r="AU15" s="12" t="s">
         <v>100</v>
@@ -4753,11 +4800,11 @@
         <v>111</v>
       </c>
       <c r="AY15" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ca="1" si="3"/>
         <v>07/07/2024</v>
       </c>
       <c r="AZ15" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ca="1" si="3"/>
         <v>07/07/2024</v>
       </c>
       <c r="BA15" s="40" t="str">
@@ -4852,9 +4899,9 @@
         <v>128</v>
       </c>
     </row>
-    <row r="16" ht="15.65" customHeight="1" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:82" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="11" t="s">
@@ -4875,7 +4922,7 @@
         <v>85</v>
       </c>
       <c r="K16" s="15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>07/07/2024</v>
       </c>
       <c r="L16" s="12" t="s">
@@ -4912,7 +4959,7 @@
         <v>85</v>
       </c>
       <c r="W16" s="15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ca="1" si="1"/>
         <v>07/07/2024</v>
       </c>
       <c r="X16" s="14" t="s">
@@ -4922,13 +4969,13 @@
         <v>93</v>
       </c>
       <c r="Z16" s="19" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="AA16" s="19" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="AB16" s="20" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="AC16" s="21">
         <v>880</v>
@@ -4946,7 +4993,7 @@
         <v>99</v>
       </c>
       <c r="AH16" s="35" t="str">
-        <f>TEXT(TODAY()+200,"DD/MM/YYYY")</f>
+        <f ca="1">TEXT(TODAY()+200,"DD/MM/YYYY")</f>
         <v>03/05/2025</v>
       </c>
       <c r="AI16" s="14" t="s">
@@ -4956,7 +5003,7 @@
         <v>102</v>
       </c>
       <c r="AK16" s="25" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="AL16" s="14" t="s">
         <v>104</v>
@@ -4977,14 +5024,14 @@
         <v>109</v>
       </c>
       <c r="AR16" s="14" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="AS16" s="14">
         <v>3</v>
       </c>
-      <c r="AT16" s="28">
-        <f t="shared" si="2"/>
-        <v>NaN</v>
+      <c r="AT16" s="28" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>07/07/2024</v>
       </c>
       <c r="AU16" s="12" t="s">
         <v>100</v>
@@ -4999,15 +5046,15 @@
         <v>111</v>
       </c>
       <c r="AY16" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ca="1" si="3"/>
         <v>07/07/2024</v>
       </c>
       <c r="AZ16" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ca="1" si="3"/>
         <v>07/07/2024</v>
       </c>
       <c r="BA16" s="35" t="str">
-        <f>TEXT(TODAY()+200,"DD/MM/YYYY")</f>
+        <f ca="1">TEXT(TODAY()+200,"DD/MM/YYYY")</f>
         <v>03/05/2025</v>
       </c>
       <c r="BB16" s="29" t="s">
@@ -5098,7 +5145,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="17" ht="15.65" customHeight="1" spans="5:32" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:82" ht="15.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E17" s="12"/>
       <c r="F17" s="13"/>
       <c r="G17" s="13"/>
@@ -5127,7 +5174,7 @@
       <c r="AE17" s="22"/>
       <c r="AF17" s="22"/>
     </row>
-    <row r="18" ht="15.65" customHeight="1" spans="27:32" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:82" ht="15.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AA18" s="19"/>
       <c r="AB18" s="36"/>
       <c r="AC18" s="19"/>
@@ -5135,7 +5182,7 @@
       <c r="AE18" s="22"/>
       <c r="AF18" s="22"/>
     </row>
-    <row r="19" ht="15.65" customHeight="1" spans="27:32" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:82" ht="15.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AA19" s="19"/>
       <c r="AB19" s="20"/>
       <c r="AC19" s="19"/>
@@ -5143,7 +5190,7 @@
       <c r="AE19" s="22"/>
       <c r="AF19" s="22"/>
     </row>
-    <row r="24" ht="15.65" customHeight="1" spans="4:82" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:82" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D24" s="35"/>
       <c r="E24" s="12"/>
       <c r="F24" s="41"/>
@@ -5224,7 +5271,7 @@
       <c r="CC24" s="29"/>
       <c r="CD24" s="29"/>
     </row>
-    <row r="25" ht="15.65" customHeight="1" spans="4:82" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:82" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D25" s="35"/>
       <c r="E25" s="12"/>
       <c r="F25" s="41"/>
@@ -5305,7 +5352,7 @@
       <c r="CC25" s="29"/>
       <c r="CD25" s="29"/>
     </row>
-    <row r="26" ht="15.65" customHeight="1" spans="4:82" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:82" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D26" s="35"/>
       <c r="E26" s="12"/>
       <c r="F26" s="41"/>
@@ -5386,7 +5433,7 @@
       <c r="CC26" s="29"/>
       <c r="CD26" s="29"/>
     </row>
-    <row r="27" ht="15.65" customHeight="1" spans="4:82" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:82" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D27" s="35"/>
       <c r="E27" s="12"/>
       <c r="F27" s="41"/>
@@ -5466,7 +5513,7 @@
       <c r="CC27" s="29"/>
       <c r="CD27" s="29"/>
     </row>
-    <row r="28" ht="15.65" customHeight="1" spans="4:82" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:82" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D28" s="35"/>
       <c r="E28" s="12"/>
       <c r="F28" s="41"/>
@@ -5547,7 +5594,7 @@
       <c r="CC28" s="29"/>
       <c r="CD28" s="29"/>
     </row>
-    <row r="29" ht="15.65" customHeight="1" spans="4:82" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:82" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D29" s="35"/>
       <c r="E29" s="12"/>
       <c r="F29" s="41"/>
@@ -5628,7 +5675,7 @@
       <c r="CC29" s="29"/>
       <c r="CD29" s="29"/>
     </row>
-    <row r="30" ht="15.65" customHeight="1" spans="4:82" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:82" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D30" s="35"/>
       <c r="E30" s="12"/>
       <c r="F30" s="41"/>
@@ -5709,7 +5756,7 @@
       <c r="CC30" s="29"/>
       <c r="CD30" s="29"/>
     </row>
-    <row r="32" ht="15.65" customHeight="1" spans="4:82" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:82" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D32" s="35"/>
       <c r="E32" s="12"/>
       <c r="F32" s="41"/>
@@ -5791,225 +5838,75 @@
       <c r="CD32" s="29"/>
     </row>
   </sheetData>
-  <dataValidations count="66">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AX10:AX16">
+  <dataValidations count="16">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AX10:AX16 X10:X17 V10:V17 S10:S17 BX10:BX16" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>INDIRECT($E2)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AX2:AX16">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AX2:AX16 X2:X17 V2:V17 S2:S17 BX2:BX16" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>INDIRECT($E2)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AX24">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AX24 X24 V24 S24 BX24" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>INDIRECT($E2)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AX25:AX26">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AX25:AX26 X32 X30 X25:X26 V32 V30 V25:V26 S32 S30 S25:S26 J8 J6 J4 J30 J2 J16 J14 J12 J10 I9 I7 I5 I32:J32 I3 I27:I30 I24:J25 I17 I15 I13 I11 BX32 BX30 BX25:BX26 AX32 AX30" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>INDIRECT(#REF!)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AX27:AX29">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AX27:AX29 X27:X29 V27:V29 S27:S29 BX27:BX29" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>INDIRECT($E2)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AX30">
-      <formula1>INDIRECT(#REF!)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AX32">
-      <formula1>INDIRECT(#REF!)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BX10:BX16">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J11" xr:uid="{00000000-0002-0000-0000-00001A000000}">
       <formula1>INDIRECT($E2)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BX2:BX16">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J13" xr:uid="{00000000-0002-0000-0000-00001C000000}">
       <formula1>INDIRECT($E2)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BX24">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J15" xr:uid="{00000000-0002-0000-0000-00001E000000}">
       <formula1>INDIRECT($E2)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BX25:BX26">
-      <formula1>INDIRECT(#REF!)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BX27:BX29">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J17" xr:uid="{00000000-0002-0000-0000-000020000000}">
       <formula1>INDIRECT($E2)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BX30">
-      <formula1>INDIRECT(#REF!)</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J26" xr:uid="{00000000-0002-0000-0000-000022000000}">
+      <formula1>INDIRECT($E6)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BX32">
-      <formula1>INDIRECT(#REF!)</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J27" xr:uid="{00000000-0002-0000-0000-000023000000}">
+      <formula1>INDIRECT($E3)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I11">
-      <formula1>INDIRECT(#REF!)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I13">
-      <formula1>INDIRECT(#REF!)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I15">
-      <formula1>INDIRECT(#REF!)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I17">
-      <formula1>INDIRECT(#REF!)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I24:J25">
-      <formula1>INDIRECT(#REF!)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I27:I30">
-      <formula1>INDIRECT(#REF!)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3">
-      <formula1>INDIRECT(#REF!)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I32:J32">
-      <formula1>INDIRECT(#REF!)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I5">
-      <formula1>INDIRECT(#REF!)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I7">
-      <formula1>INDIRECT(#REF!)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I9">
-      <formula1>INDIRECT(#REF!)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J10">
-      <formula1>INDIRECT(#REF!)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J28:J29" xr:uid="{00000000-0002-0000-0000-000024000000}">
       <formula1>INDIRECT($E2)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J12">
-      <formula1>INDIRECT(#REF!)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J3" xr:uid="{00000000-0002-0000-0000-000025000000}">
       <formula1>INDIRECT($E2)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J14">
-      <formula1>INDIRECT(#REF!)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J5" xr:uid="{00000000-0002-0000-0000-000028000000}">
       <formula1>INDIRECT($E2)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J16">
-      <formula1>INDIRECT(#REF!)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J17">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J7" xr:uid="{00000000-0002-0000-0000-00002A000000}">
       <formula1>INDIRECT($E2)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2">
-      <formula1>INDIRECT(#REF!)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J26">
-      <formula1>INDIRECT($E6)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J27">
-      <formula1>INDIRECT($E3)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J28:J29">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J9" xr:uid="{00000000-0002-0000-0000-00002C000000}">
       <formula1>INDIRECT($E2)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J3">
-      <formula1>INDIRECT($E2)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J30">
-      <formula1>INDIRECT(#REF!)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J4">
-      <formula1>INDIRECT(#REF!)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J5">
-      <formula1>INDIRECT($E2)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J6">
-      <formula1>INDIRECT(#REF!)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J7">
-      <formula1>INDIRECT($E2)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J8">
-      <formula1>INDIRECT(#REF!)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J9">
-      <formula1>INDIRECT($E2)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S10:S17">
-      <formula1>INDIRECT($E2)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2:S17">
-      <formula1>INDIRECT($E2)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S24">
-      <formula1>INDIRECT($E2)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S25:S26">
-      <formula1>INDIRECT(#REF!)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S27:S29">
-      <formula1>INDIRECT($E2)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S30">
-      <formula1>INDIRECT(#REF!)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S32">
-      <formula1>INDIRECT(#REF!)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V10:V17">
-      <formula1>INDIRECT($E2)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V2:V17">
-      <formula1>INDIRECT($E2)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V24">
-      <formula1>INDIRECT($E2)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V25:V26">
-      <formula1>INDIRECT(#REF!)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V27:V29">
-      <formula1>INDIRECT($E2)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V30">
-      <formula1>INDIRECT(#REF!)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V32">
-      <formula1>INDIRECT(#REF!)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X10:X17">
-      <formula1>INDIRECT($E2)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X2:X17">
-      <formula1>INDIRECT($E2)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X24">
-      <formula1>INDIRECT($E2)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X25:X26">
-      <formula1>INDIRECT(#REF!)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X27:X29">
-      <formula1>INDIRECT($E2)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X30">
-      <formula1>INDIRECT(#REF!)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X32">
-      <formula1>INDIRECT(#REF!)</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="U2" r:id="rId1"/>
-    <hyperlink ref="U3" r:id="rId2"/>
-    <hyperlink ref="U4" r:id="rId3"/>
-    <hyperlink ref="U5" r:id="rId4"/>
-    <hyperlink ref="U6" r:id="rId5"/>
-    <hyperlink ref="U7" r:id="rId6"/>
-    <hyperlink ref="U8" r:id="rId7"/>
-    <hyperlink ref="U9" r:id="rId8"/>
-    <hyperlink ref="U10" r:id="rId9"/>
-    <hyperlink ref="U11" r:id="rId10"/>
-    <hyperlink ref="U12" r:id="rId11"/>
-    <hyperlink ref="U13" r:id="rId12"/>
-    <hyperlink ref="U14" r:id="rId13"/>
-    <hyperlink ref="U15" r:id="rId14"/>
-    <hyperlink ref="U16" r:id="rId15"/>
+    <hyperlink ref="U2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="U3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="U4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="U5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="U6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="U7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="U8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="U9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="U10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="U11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="U12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="U13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="U14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="U15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="U16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="4294967295"/>
   <headerFooter>
     <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 EXPLEO Internal</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Changes on the US Hire process
</commit_message>
<xml_diff>
--- a/Data/testDataRomania.xlsx
+++ b/Data/testDataRomania.xlsx
@@ -1,30 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{62C1033C-6C4C-4C47-8D90-446003281065}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
+    <sheet sheetId="1" name="Sheet2" state="visible" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -427,10 +412,10 @@
 </t>
   </si>
   <si>
-    <t>Kenna</t>
-  </si>
-  <si>
-    <t>Balistreri</t>
+    <t>Eunice</t>
+  </si>
+  <si>
+    <t>Feest</t>
   </si>
   <si>
     <t>Fixed Term (Fixed Term)</t>
@@ -454,7 +439,7 @@
     <t>Store Manager_NEW</t>
   </si>
   <si>
-    <t>92 Retail Management </t>
+    <t xml:space="preserve">92 Retail Management </t>
   </si>
   <si>
     <t>251 Management Retail</t>
@@ -554,51 +539,51 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
     <font>
+      <family val="2"/>
+      <scheme val="minor"/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <color theme="4"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color theme="4"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <u/>
+      <family val="2"/>
+      <scheme val="minor"/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <color rgb="FF000000"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -610,7 +595,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
+        <fgColor theme="5" tint="0.5999938962981048"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -635,12 +620,8 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
     <border>
@@ -650,27 +631,17 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
+      <top style="thin"/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
@@ -1093,14 +1064,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CD32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.65" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.65" outlineLevelRow="1" outlineLevelCol="0" x14ac:dyDescent="0.35" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="10.81640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="11.81640625" style="1" customWidth="1"/>
@@ -1186,7 +1157,7 @@
     <col min="83" max="83" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:82" s="3" customFormat="1" ht="14.5" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="1" ht="14.5" customHeight="1" spans="1:82" s="3" customFormat="1" x14ac:dyDescent="0.25" outlineLevel="1" collapsed="1">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1434,7 +1405,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:82" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" ht="15.65" customHeight="1" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>77</v>
       </c>
@@ -1466,7 +1437,7 @@
         <v>85</v>
       </c>
       <c r="K2" s="15" t="str">
-        <f t="shared" ref="K2:K16" ca="1" si="0">TEXT(TODAY()-100,"DD/MM/YYYY")</f>
+        <f t="shared" ref="K2:K16" si="0">TEXT(TODAY()-100,"DD/MM/YYYY")</f>
         <v>07/07/2024</v>
       </c>
       <c r="L2" s="12" t="s">
@@ -1503,7 +1474,7 @@
         <v>85</v>
       </c>
       <c r="W2" s="15" t="str">
-        <f t="shared" ref="W2:W16" ca="1" si="1">TEXT(TODAY()-100,"DD/MM/YYYY")</f>
+        <f t="shared" ref="W2:W16" si="1">TEXT(TODAY()-100,"DD/MM/YYYY")</f>
         <v>07/07/2024</v>
       </c>
       <c r="X2" s="14" t="s">
@@ -1572,9 +1543,9 @@
       <c r="AS2" s="14">
         <v>1</v>
       </c>
-      <c r="AT2" s="28" t="str">
-        <f t="shared" ref="AT2:AT16" ca="1" si="2">TEXT(TODAY()-100,"DD/MM/YYYY")</f>
-        <v>07/07/2024</v>
+      <c r="AT2" s="28">
+        <f t="shared" ref="AT2:AT16" si="2">TEXT(TODAY()-100,"DD/MM/YYYY")</f>
+        <v>NaN</v>
       </c>
       <c r="AU2" s="12" t="s">
         <v>100</v>
@@ -1589,11 +1560,11 @@
         <v>111</v>
       </c>
       <c r="AY2" s="15" t="str">
-        <f t="shared" ref="AY2:AZ16" ca="1" si="3">TEXT(TODAY()-100,"DD/MM/YYYY")</f>
+        <f t="shared" ref="AY2:AZ16" si="3">TEXT(TODAY()-100,"DD/MM/YYYY")</f>
         <v>07/07/2024</v>
       </c>
       <c r="AZ2" s="15" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>07/07/2024</v>
       </c>
       <c r="BA2" s="24" t="s">
@@ -1687,7 +1658,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="3" spans="1:82" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" ht="15.65" customHeight="1" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>129</v>
       </c>
@@ -1719,7 +1690,7 @@
         <v>85</v>
       </c>
       <c r="K3" s="15" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>07/07/2024</v>
       </c>
       <c r="L3" s="32" t="s">
@@ -1756,7 +1727,7 @@
         <v>85</v>
       </c>
       <c r="W3" s="15" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" si="1"/>
         <v>07/07/2024</v>
       </c>
       <c r="X3" s="14" t="s">
@@ -1790,7 +1761,7 @@
         <v>99</v>
       </c>
       <c r="AH3" s="35" t="str">
-        <f t="shared" ref="AH3:AH5" ca="1" si="4">TEXT(TODAY()+200,"DD/MM/YYYY")</f>
+        <f t="shared" ref="AH3:AH5" si="4">TEXT(TODAY()+200,"DD/MM/YYYY")</f>
         <v>03/05/2025</v>
       </c>
       <c r="AI3" s="14" t="s">
@@ -1826,9 +1797,9 @@
       <c r="AS3" s="14">
         <v>2</v>
       </c>
-      <c r="AT3" s="28" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>07/07/2024</v>
+      <c r="AT3" s="28">
+        <f t="shared" si="2"/>
+        <v>NaN</v>
       </c>
       <c r="AU3" s="12" t="s">
         <v>100</v>
@@ -1843,15 +1814,15 @@
         <v>111</v>
       </c>
       <c r="AY3" s="15" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>07/07/2024</v>
       </c>
       <c r="AZ3" s="15" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>07/07/2024</v>
       </c>
       <c r="BA3" s="35" t="str">
-        <f ca="1">TEXT(TODAY()+200,"DD/MM/YYYY")</f>
+        <f>TEXT(TODAY()+200,"DD/MM/YYYY")</f>
         <v>03/05/2025</v>
       </c>
       <c r="BB3" s="29" t="s">
@@ -1942,7 +1913,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="1:82" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" ht="15.65" customHeight="1" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>136</v>
       </c>
@@ -1968,7 +1939,7 @@
         <v>85</v>
       </c>
       <c r="K4" s="15" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>07/07/2024</v>
       </c>
       <c r="L4" s="12" t="s">
@@ -2005,7 +1976,7 @@
         <v>85</v>
       </c>
       <c r="W4" s="15" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" si="1"/>
         <v>07/07/2024</v>
       </c>
       <c r="X4" s="14" t="s">
@@ -2039,7 +2010,7 @@
         <v>99</v>
       </c>
       <c r="AH4" s="35" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="4"/>
         <v>03/05/2025</v>
       </c>
       <c r="AI4" s="14" t="s">
@@ -2075,9 +2046,9 @@
       <c r="AS4" s="14">
         <v>3</v>
       </c>
-      <c r="AT4" s="28" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>07/07/2024</v>
+      <c r="AT4" s="28">
+        <f t="shared" si="2"/>
+        <v>NaN</v>
       </c>
       <c r="AU4" s="12" t="s">
         <v>100</v>
@@ -2092,15 +2063,15 @@
         <v>111</v>
       </c>
       <c r="AY4" s="15" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>07/07/2024</v>
       </c>
       <c r="AZ4" s="15" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>07/07/2024</v>
       </c>
       <c r="BA4" s="35" t="str">
-        <f t="shared" ref="BA4:BA5" ca="1" si="5">TEXT(TODAY()+200,"DD/MM/YYYY")</f>
+        <f t="shared" ref="BA4:BA5" si="5">TEXT(TODAY()+200,"DD/MM/YYYY")</f>
         <v>03/05/2025</v>
       </c>
       <c r="BB4" s="29" t="s">
@@ -2191,7 +2162,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:82" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" ht="15.65" customHeight="1" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>142</v>
       </c>
@@ -2217,7 +2188,7 @@
         <v>85</v>
       </c>
       <c r="K5" s="15" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>07/07/2024</v>
       </c>
       <c r="L5" s="32" t="s">
@@ -2254,7 +2225,7 @@
         <v>85</v>
       </c>
       <c r="W5" s="15" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" si="1"/>
         <v>07/07/2024</v>
       </c>
       <c r="X5" s="14" t="s">
@@ -2288,7 +2259,7 @@
         <v>99</v>
       </c>
       <c r="AH5" s="35" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="4"/>
         <v>03/05/2025</v>
       </c>
       <c r="AI5" s="14" t="s">
@@ -2324,9 +2295,9 @@
       <c r="AS5" s="14">
         <v>1</v>
       </c>
-      <c r="AT5" s="28" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>07/07/2024</v>
+      <c r="AT5" s="28">
+        <f t="shared" si="2"/>
+        <v>NaN</v>
       </c>
       <c r="AU5" s="12" t="s">
         <v>100</v>
@@ -2341,15 +2312,15 @@
         <v>111</v>
       </c>
       <c r="AY5" s="15" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>07/07/2024</v>
       </c>
       <c r="AZ5" s="15" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>07/07/2024</v>
       </c>
       <c r="BA5" s="35" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>03/05/2025</v>
       </c>
       <c r="BB5" s="29" t="s">
@@ -2440,7 +2411,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="6" spans="1:82" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" ht="15.65" customHeight="1" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>145</v>
       </c>
@@ -2464,7 +2435,7 @@
         <v>85</v>
       </c>
       <c r="K6" s="15" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>07/07/2024</v>
       </c>
       <c r="L6" s="12" t="s">
@@ -2501,7 +2472,7 @@
         <v>85</v>
       </c>
       <c r="W6" s="15" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" si="1"/>
         <v>07/07/2024</v>
       </c>
       <c r="X6" s="14" t="s">
@@ -2570,9 +2541,9 @@
       <c r="AS6" s="14">
         <v>2</v>
       </c>
-      <c r="AT6" s="28" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>07/07/2024</v>
+      <c r="AT6" s="28">
+        <f t="shared" si="2"/>
+        <v>NaN</v>
       </c>
       <c r="AU6" s="12" t="s">
         <v>100</v>
@@ -2587,11 +2558,11 @@
         <v>111</v>
       </c>
       <c r="AY6" s="15" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>07/07/2024</v>
       </c>
       <c r="AZ6" s="15" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>07/07/2024</v>
       </c>
       <c r="BA6" s="24" t="str">
@@ -2686,7 +2657,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="7" spans="1:82" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" ht="15.65" customHeight="1" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>148</v>
       </c>
@@ -2710,7 +2681,7 @@
         <v>85</v>
       </c>
       <c r="K7" s="15" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>07/07/2024</v>
       </c>
       <c r="L7" s="32" t="s">
@@ -2747,7 +2718,7 @@
         <v>85</v>
       </c>
       <c r="W7" s="15" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" si="1"/>
         <v>07/07/2024</v>
       </c>
       <c r="X7" s="14" t="s">
@@ -2781,7 +2752,7 @@
         <v>99</v>
       </c>
       <c r="AH7" s="35" t="str">
-        <f ca="1">TEXT(TODAY()+200,"DD/MM/YYYY")</f>
+        <f>TEXT(TODAY()+200,"DD/MM/YYYY")</f>
         <v>03/05/2025</v>
       </c>
       <c r="AI7" s="14" t="s">
@@ -2817,9 +2788,9 @@
       <c r="AS7" s="14">
         <v>3</v>
       </c>
-      <c r="AT7" s="28" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>07/07/2024</v>
+      <c r="AT7" s="28">
+        <f t="shared" si="2"/>
+        <v>NaN</v>
       </c>
       <c r="AU7" s="12" t="s">
         <v>100</v>
@@ -2834,15 +2805,15 @@
         <v>111</v>
       </c>
       <c r="AY7" s="15" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>07/07/2024</v>
       </c>
       <c r="AZ7" s="15" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>07/07/2024</v>
       </c>
       <c r="BA7" s="35" t="str">
-        <f ca="1">TEXT(TODAY()+200,"DD/MM/YYYY")</f>
+        <f>TEXT(TODAY()+200,"DD/MM/YYYY")</f>
         <v>03/05/2025</v>
       </c>
       <c r="BB7" s="29" t="s">
@@ -2933,7 +2904,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="8" spans="1:82" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" ht="15.65" customHeight="1" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>151</v>
       </c>
@@ -2957,7 +2928,7 @@
         <v>85</v>
       </c>
       <c r="K8" s="15" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>07/07/2024</v>
       </c>
       <c r="L8" s="12" t="s">
@@ -2994,7 +2965,7 @@
         <v>85</v>
       </c>
       <c r="W8" s="15" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" si="1"/>
         <v>07/07/2024</v>
       </c>
       <c r="X8" s="14" t="s">
@@ -3063,9 +3034,9 @@
       <c r="AS8" s="14">
         <v>1</v>
       </c>
-      <c r="AT8" s="28" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>07/07/2024</v>
+      <c r="AT8" s="28">
+        <f t="shared" si="2"/>
+        <v>NaN</v>
       </c>
       <c r="AU8" s="12" t="s">
         <v>100</v>
@@ -3080,11 +3051,11 @@
         <v>111</v>
       </c>
       <c r="AY8" s="15" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>07/07/2024</v>
       </c>
       <c r="AZ8" s="15" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>07/07/2024</v>
       </c>
       <c r="BA8" s="24" t="str">
@@ -3179,7 +3150,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="9" spans="1:82" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" ht="15.65" customHeight="1" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>154</v>
       </c>
@@ -3203,7 +3174,7 @@
         <v>85</v>
       </c>
       <c r="K9" s="15" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>07/07/2024</v>
       </c>
       <c r="L9" s="32" t="s">
@@ -3240,7 +3211,7 @@
         <v>85</v>
       </c>
       <c r="W9" s="15" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" si="1"/>
         <v>07/07/2024</v>
       </c>
       <c r="X9" s="14" t="s">
@@ -3274,7 +3245,7 @@
         <v>99</v>
       </c>
       <c r="AH9" s="35" t="str">
-        <f ca="1">TEXT(TODAY()+200,"DD/MM/YYYY")</f>
+        <f>TEXT(TODAY()+200,"DD/MM/YYYY")</f>
         <v>03/05/2025</v>
       </c>
       <c r="AI9" s="14" t="s">
@@ -3310,9 +3281,9 @@
       <c r="AS9" s="14">
         <v>2</v>
       </c>
-      <c r="AT9" s="28" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>07/07/2024</v>
+      <c r="AT9" s="28">
+        <f t="shared" si="2"/>
+        <v>NaN</v>
       </c>
       <c r="AU9" s="12" t="s">
         <v>100</v>
@@ -3327,15 +3298,15 @@
         <v>111</v>
       </c>
       <c r="AY9" s="15" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>07/07/2024</v>
       </c>
       <c r="AZ9" s="15" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>07/07/2024</v>
       </c>
       <c r="BA9" s="35" t="str">
-        <f ca="1">TEXT(TODAY()+200,"DD/MM/YYYY")</f>
+        <f>TEXT(TODAY()+200,"DD/MM/YYYY")</f>
         <v>03/05/2025</v>
       </c>
       <c r="BB9" s="29" t="s">
@@ -3426,7 +3397,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="10" spans="1:82" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" ht="15.65" customHeight="1" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>157</v>
       </c>
@@ -3449,7 +3420,7 @@
         <v>85</v>
       </c>
       <c r="K10" s="15" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>07/07/2024</v>
       </c>
       <c r="L10" s="12" t="s">
@@ -3486,7 +3457,7 @@
         <v>85</v>
       </c>
       <c r="W10" s="15" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" si="1"/>
         <v>07/07/2024</v>
       </c>
       <c r="X10" s="14" t="s">
@@ -3555,9 +3526,9 @@
       <c r="AS10" s="14">
         <v>3</v>
       </c>
-      <c r="AT10" s="28" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>07/07/2024</v>
+      <c r="AT10" s="28">
+        <f t="shared" si="2"/>
+        <v>NaN</v>
       </c>
       <c r="AU10" s="12" t="s">
         <v>100</v>
@@ -3572,11 +3543,11 @@
         <v>111</v>
       </c>
       <c r="AY10" s="15" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>07/07/2024</v>
       </c>
       <c r="AZ10" s="15" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>07/07/2024</v>
       </c>
       <c r="BA10" s="40" t="str">
@@ -3671,7 +3642,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="11" spans="1:82" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" ht="15.65" customHeight="1" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>161</v>
       </c>
@@ -3694,7 +3665,7 @@
         <v>85</v>
       </c>
       <c r="K11" s="15" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>07/07/2024</v>
       </c>
       <c r="L11" s="32" t="s">
@@ -3731,7 +3702,7 @@
         <v>85</v>
       </c>
       <c r="W11" s="15" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" si="1"/>
         <v>07/07/2024</v>
       </c>
       <c r="X11" s="14" t="s">
@@ -3765,7 +3736,7 @@
         <v>99</v>
       </c>
       <c r="AH11" s="35" t="str">
-        <f ca="1">TEXT(TODAY()+200,"DD/MM/YYYY")</f>
+        <f>TEXT(TODAY()+200,"DD/MM/YYYY")</f>
         <v>03/05/2025</v>
       </c>
       <c r="AI11" s="14" t="s">
@@ -3801,9 +3772,9 @@
       <c r="AS11" s="14">
         <v>1</v>
       </c>
-      <c r="AT11" s="28" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>07/07/2024</v>
+      <c r="AT11" s="28">
+        <f t="shared" si="2"/>
+        <v>NaN</v>
       </c>
       <c r="AU11" s="12" t="s">
         <v>100</v>
@@ -3818,15 +3789,15 @@
         <v>111</v>
       </c>
       <c r="AY11" s="15" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>07/07/2024</v>
       </c>
       <c r="AZ11" s="15" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>07/07/2024</v>
       </c>
       <c r="BA11" s="35" t="str">
-        <f ca="1">TEXT(TODAY()+200,"DD/MM/YYYY")</f>
+        <f>TEXT(TODAY()+200,"DD/MM/YYYY")</f>
         <v>03/05/2025</v>
       </c>
       <c r="BB11" s="29" t="s">
@@ -3917,7 +3888,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="12" spans="1:82" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" ht="15.65" customHeight="1" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>164</v>
       </c>
@@ -3940,7 +3911,7 @@
         <v>85</v>
       </c>
       <c r="K12" s="15" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>07/07/2024</v>
       </c>
       <c r="L12" s="12" t="s">
@@ -3977,7 +3948,7 @@
         <v>85</v>
       </c>
       <c r="W12" s="15" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" si="1"/>
         <v>07/07/2024</v>
       </c>
       <c r="X12" s="14" t="s">
@@ -4046,9 +4017,9 @@
       <c r="AS12" s="14">
         <v>2</v>
       </c>
-      <c r="AT12" s="28" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>07/07/2024</v>
+      <c r="AT12" s="28">
+        <f t="shared" si="2"/>
+        <v>NaN</v>
       </c>
       <c r="AU12" s="12" t="s">
         <v>100</v>
@@ -4063,11 +4034,11 @@
         <v>111</v>
       </c>
       <c r="AY12" s="15" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>07/07/2024</v>
       </c>
       <c r="AZ12" s="15" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>07/07/2024</v>
       </c>
       <c r="BA12" s="40" t="str">
@@ -4162,7 +4133,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="13" spans="1:82" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" ht="15.65" customHeight="1" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>166</v>
       </c>
@@ -4185,7 +4156,7 @@
         <v>85</v>
       </c>
       <c r="K13" s="15" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>07/07/2024</v>
       </c>
       <c r="L13" s="32" t="s">
@@ -4222,7 +4193,7 @@
         <v>85</v>
       </c>
       <c r="W13" s="15" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" si="1"/>
         <v>07/07/2024</v>
       </c>
       <c r="X13" s="14" t="s">
@@ -4256,7 +4227,7 @@
         <v>99</v>
       </c>
       <c r="AH13" s="35" t="str">
-        <f ca="1">TEXT(TODAY()+200,"DD/MM/YYYY")</f>
+        <f>TEXT(TODAY()+200,"DD/MM/YYYY")</f>
         <v>03/05/2025</v>
       </c>
       <c r="AI13" s="14" t="s">
@@ -4292,9 +4263,9 @@
       <c r="AS13" s="14">
         <v>3</v>
       </c>
-      <c r="AT13" s="28" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>07/07/2024</v>
+      <c r="AT13" s="28">
+        <f t="shared" si="2"/>
+        <v>NaN</v>
       </c>
       <c r="AU13" s="12" t="s">
         <v>100</v>
@@ -4309,15 +4280,15 @@
         <v>111</v>
       </c>
       <c r="AY13" s="15" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>07/07/2024</v>
       </c>
       <c r="AZ13" s="15" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>07/07/2024</v>
       </c>
       <c r="BA13" s="35" t="str">
-        <f ca="1">TEXT(TODAY()+200,"DD/MM/YYYY")</f>
+        <f>TEXT(TODAY()+200,"DD/MM/YYYY")</f>
         <v>03/05/2025</v>
       </c>
       <c r="BB13" s="29" t="s">
@@ -4408,7 +4379,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="14" spans="1:82" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" ht="15.65" customHeight="1" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>168</v>
       </c>
@@ -4432,7 +4403,7 @@
         <v>85</v>
       </c>
       <c r="K14" s="15" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>07/07/2024</v>
       </c>
       <c r="L14" s="12" t="s">
@@ -4469,7 +4440,7 @@
         <v>85</v>
       </c>
       <c r="W14" s="15" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" si="1"/>
         <v>07/07/2024</v>
       </c>
       <c r="X14" s="14" t="s">
@@ -4538,9 +4509,9 @@
       <c r="AS14" s="14">
         <v>1</v>
       </c>
-      <c r="AT14" s="28" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>07/07/2024</v>
+      <c r="AT14" s="28">
+        <f t="shared" si="2"/>
+        <v>NaN</v>
       </c>
       <c r="AU14" s="12" t="s">
         <v>100</v>
@@ -4555,11 +4526,11 @@
         <v>111</v>
       </c>
       <c r="AY14" s="15" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>07/07/2024</v>
       </c>
       <c r="AZ14" s="15" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>07/07/2024</v>
       </c>
       <c r="BA14" s="40" t="str">
@@ -4654,7 +4625,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="15" spans="1:82" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" ht="15.65" customHeight="1" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>169</v>
       </c>
@@ -4677,7 +4648,7 @@
         <v>85</v>
       </c>
       <c r="K15" s="15" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>07/07/2024</v>
       </c>
       <c r="L15" s="32" t="s">
@@ -4714,7 +4685,7 @@
         <v>85</v>
       </c>
       <c r="W15" s="15" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" si="1"/>
         <v>07/07/2024</v>
       </c>
       <c r="X15" s="14" t="s">
@@ -4783,9 +4754,9 @@
       <c r="AS15" s="14">
         <v>2</v>
       </c>
-      <c r="AT15" s="28" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>07/07/2024</v>
+      <c r="AT15" s="28">
+        <f t="shared" si="2"/>
+        <v>NaN</v>
       </c>
       <c r="AU15" s="12" t="s">
         <v>100</v>
@@ -4800,11 +4771,11 @@
         <v>111</v>
       </c>
       <c r="AY15" s="15" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>07/07/2024</v>
       </c>
       <c r="AZ15" s="15" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>07/07/2024</v>
       </c>
       <c r="BA15" s="40" t="str">
@@ -4899,7 +4870,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="16" spans="1:82" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" ht="15.65" customHeight="1" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>171</v>
       </c>
@@ -4922,7 +4893,7 @@
         <v>85</v>
       </c>
       <c r="K16" s="15" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>07/07/2024</v>
       </c>
       <c r="L16" s="12" t="s">
@@ -4959,7 +4930,7 @@
         <v>85</v>
       </c>
       <c r="W16" s="15" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" si="1"/>
         <v>07/07/2024</v>
       </c>
       <c r="X16" s="14" t="s">
@@ -4993,7 +4964,7 @@
         <v>99</v>
       </c>
       <c r="AH16" s="35" t="str">
-        <f ca="1">TEXT(TODAY()+200,"DD/MM/YYYY")</f>
+        <f>TEXT(TODAY()+200,"DD/MM/YYYY")</f>
         <v>03/05/2025</v>
       </c>
       <c r="AI16" s="14" t="s">
@@ -5029,9 +5000,9 @@
       <c r="AS16" s="14">
         <v>3</v>
       </c>
-      <c r="AT16" s="28" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>07/07/2024</v>
+      <c r="AT16" s="28">
+        <f t="shared" si="2"/>
+        <v>NaN</v>
       </c>
       <c r="AU16" s="12" t="s">
         <v>100</v>
@@ -5046,15 +5017,15 @@
         <v>111</v>
       </c>
       <c r="AY16" s="15" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>07/07/2024</v>
       </c>
       <c r="AZ16" s="15" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>07/07/2024</v>
       </c>
       <c r="BA16" s="35" t="str">
-        <f ca="1">TEXT(TODAY()+200,"DD/MM/YYYY")</f>
+        <f>TEXT(TODAY()+200,"DD/MM/YYYY")</f>
         <v>03/05/2025</v>
       </c>
       <c r="BB16" s="29" t="s">
@@ -5145,7 +5116,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="17" spans="4:82" ht="15.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" ht="15.65" customHeight="1" spans="5:32" x14ac:dyDescent="0.25">
       <c r="E17" s="12"/>
       <c r="F17" s="13"/>
       <c r="G17" s="13"/>
@@ -5174,7 +5145,7 @@
       <c r="AE17" s="22"/>
       <c r="AF17" s="22"/>
     </row>
-    <row r="18" spans="4:82" ht="15.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" ht="15.65" customHeight="1" spans="27:32" x14ac:dyDescent="0.25">
       <c r="AA18" s="19"/>
       <c r="AB18" s="36"/>
       <c r="AC18" s="19"/>
@@ -5182,7 +5153,7 @@
       <c r="AE18" s="22"/>
       <c r="AF18" s="22"/>
     </row>
-    <row r="19" spans="4:82" ht="15.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" ht="15.65" customHeight="1" spans="27:32" x14ac:dyDescent="0.25">
       <c r="AA19" s="19"/>
       <c r="AB19" s="20"/>
       <c r="AC19" s="19"/>
@@ -5190,7 +5161,7 @@
       <c r="AE19" s="22"/>
       <c r="AF19" s="22"/>
     </row>
-    <row r="24" spans="4:82" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" ht="15.65" customHeight="1" spans="4:82" x14ac:dyDescent="0.25">
       <c r="D24" s="35"/>
       <c r="E24" s="12"/>
       <c r="F24" s="41"/>
@@ -5271,7 +5242,7 @@
       <c r="CC24" s="29"/>
       <c r="CD24" s="29"/>
     </row>
-    <row r="25" spans="4:82" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" ht="15.65" customHeight="1" spans="4:82" x14ac:dyDescent="0.25">
       <c r="D25" s="35"/>
       <c r="E25" s="12"/>
       <c r="F25" s="41"/>
@@ -5352,7 +5323,7 @@
       <c r="CC25" s="29"/>
       <c r="CD25" s="29"/>
     </row>
-    <row r="26" spans="4:82" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" ht="15.65" customHeight="1" spans="4:82" x14ac:dyDescent="0.25">
       <c r="D26" s="35"/>
       <c r="E26" s="12"/>
       <c r="F26" s="41"/>
@@ -5433,7 +5404,7 @@
       <c r="CC26" s="29"/>
       <c r="CD26" s="29"/>
     </row>
-    <row r="27" spans="4:82" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" ht="15.65" customHeight="1" spans="4:82" x14ac:dyDescent="0.25">
       <c r="D27" s="35"/>
       <c r="E27" s="12"/>
       <c r="F27" s="41"/>
@@ -5513,7 +5484,7 @@
       <c r="CC27" s="29"/>
       <c r="CD27" s="29"/>
     </row>
-    <row r="28" spans="4:82" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" ht="15.65" customHeight="1" spans="4:82" x14ac:dyDescent="0.25">
       <c r="D28" s="35"/>
       <c r="E28" s="12"/>
       <c r="F28" s="41"/>
@@ -5594,7 +5565,7 @@
       <c r="CC28" s="29"/>
       <c r="CD28" s="29"/>
     </row>
-    <row r="29" spans="4:82" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" ht="15.65" customHeight="1" spans="4:82" x14ac:dyDescent="0.25">
       <c r="D29" s="35"/>
       <c r="E29" s="12"/>
       <c r="F29" s="41"/>
@@ -5675,7 +5646,7 @@
       <c r="CC29" s="29"/>
       <c r="CD29" s="29"/>
     </row>
-    <row r="30" spans="4:82" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" ht="15.65" customHeight="1" spans="4:82" x14ac:dyDescent="0.25">
       <c r="D30" s="35"/>
       <c r="E30" s="12"/>
       <c r="F30" s="41"/>
@@ -5756,7 +5727,7 @@
       <c r="CC30" s="29"/>
       <c r="CD30" s="29"/>
     </row>
-    <row r="32" spans="4:82" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" ht="15.65" customHeight="1" spans="4:82" x14ac:dyDescent="0.25">
       <c r="D32" s="35"/>
       <c r="E32" s="12"/>
       <c r="F32" s="41"/>
@@ -5838,75 +5809,225 @@
       <c r="CD32" s="29"/>
     </row>
   </sheetData>
-  <dataValidations count="16">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AX10:AX16 X10:X17 V10:V17 S10:S17 BX10:BX16" xr:uid="{00000000-0002-0000-0000-000000000000}">
+  <dataValidations count="66">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AX10:AX16">
       <formula1>INDIRECT($E2)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AX2:AX16 X2:X17 V2:V17 S2:S17 BX2:BX16" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AX2:AX16">
       <formula1>INDIRECT($E2)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AX24 X24 V24 S24 BX24" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AX24">
       <formula1>INDIRECT($E2)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AX25:AX26 X32 X30 X25:X26 V32 V30 V25:V26 S32 S30 S25:S26 J8 J6 J4 J30 J2 J16 J14 J12 J10 I9 I7 I5 I32:J32 I3 I27:I30 I24:J25 I17 I15 I13 I11 BX32 BX30 BX25:BX26 AX32 AX30" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AX25:AX26">
       <formula1>INDIRECT(#REF!)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AX27:AX29 X27:X29 V27:V29 S27:S29 BX27:BX29" xr:uid="{00000000-0002-0000-0000-000004000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AX27:AX29">
       <formula1>INDIRECT($E2)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J11" xr:uid="{00000000-0002-0000-0000-00001A000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AX30">
+      <formula1>INDIRECT(#REF!)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AX32">
+      <formula1>INDIRECT(#REF!)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BX10:BX16">
       <formula1>INDIRECT($E2)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J13" xr:uid="{00000000-0002-0000-0000-00001C000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BX2:BX16">
       <formula1>INDIRECT($E2)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J15" xr:uid="{00000000-0002-0000-0000-00001E000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BX24">
       <formula1>INDIRECT($E2)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J17" xr:uid="{00000000-0002-0000-0000-000020000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BX25:BX26">
+      <formula1>INDIRECT(#REF!)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BX27:BX29">
       <formula1>INDIRECT($E2)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J26" xr:uid="{00000000-0002-0000-0000-000022000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BX30">
+      <formula1>INDIRECT(#REF!)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BX32">
+      <formula1>INDIRECT(#REF!)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I11">
+      <formula1>INDIRECT(#REF!)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I13">
+      <formula1>INDIRECT(#REF!)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I15">
+      <formula1>INDIRECT(#REF!)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I17">
+      <formula1>INDIRECT(#REF!)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I24:J25">
+      <formula1>INDIRECT(#REF!)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I27:I30">
+      <formula1>INDIRECT(#REF!)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3">
+      <formula1>INDIRECT(#REF!)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I32:J32">
+      <formula1>INDIRECT(#REF!)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I5">
+      <formula1>INDIRECT(#REF!)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I7">
+      <formula1>INDIRECT(#REF!)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I9">
+      <formula1>INDIRECT(#REF!)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J10">
+      <formula1>INDIRECT(#REF!)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J11">
+      <formula1>INDIRECT($E2)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J12">
+      <formula1>INDIRECT(#REF!)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J13">
+      <formula1>INDIRECT($E2)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J14">
+      <formula1>INDIRECT(#REF!)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J15">
+      <formula1>INDIRECT($E2)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J16">
+      <formula1>INDIRECT(#REF!)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J17">
+      <formula1>INDIRECT($E2)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2">
+      <formula1>INDIRECT(#REF!)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J26">
       <formula1>INDIRECT($E6)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J27" xr:uid="{00000000-0002-0000-0000-000023000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J27">
       <formula1>INDIRECT($E3)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J28:J29" xr:uid="{00000000-0002-0000-0000-000024000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J28:J29">
       <formula1>INDIRECT($E2)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J3" xr:uid="{00000000-0002-0000-0000-000025000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J3">
       <formula1>INDIRECT($E2)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J5" xr:uid="{00000000-0002-0000-0000-000028000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J30">
+      <formula1>INDIRECT(#REF!)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J4">
+      <formula1>INDIRECT(#REF!)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J5">
       <formula1>INDIRECT($E2)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J7" xr:uid="{00000000-0002-0000-0000-00002A000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J6">
+      <formula1>INDIRECT(#REF!)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J7">
       <formula1>INDIRECT($E2)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J9" xr:uid="{00000000-0002-0000-0000-00002C000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J8">
+      <formula1>INDIRECT(#REF!)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J9">
       <formula1>INDIRECT($E2)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S10:S17">
+      <formula1>INDIRECT($E2)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2:S17">
+      <formula1>INDIRECT($E2)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S24">
+      <formula1>INDIRECT($E2)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S25:S26">
+      <formula1>INDIRECT(#REF!)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S27:S29">
+      <formula1>INDIRECT($E2)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S30">
+      <formula1>INDIRECT(#REF!)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S32">
+      <formula1>INDIRECT(#REF!)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V10:V17">
+      <formula1>INDIRECT($E2)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V2:V17">
+      <formula1>INDIRECT($E2)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V24">
+      <formula1>INDIRECT($E2)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V25:V26">
+      <formula1>INDIRECT(#REF!)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V27:V29">
+      <formula1>INDIRECT($E2)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V30">
+      <formula1>INDIRECT(#REF!)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V32">
+      <formula1>INDIRECT(#REF!)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X10:X17">
+      <formula1>INDIRECT($E2)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X2:X17">
+      <formula1>INDIRECT($E2)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X24">
+      <formula1>INDIRECT($E2)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X25:X26">
+      <formula1>INDIRECT(#REF!)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X27:X29">
+      <formula1>INDIRECT($E2)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X30">
+      <formula1>INDIRECT(#REF!)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X32">
+      <formula1>INDIRECT(#REF!)</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="U2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="U3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="U4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="U5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="U6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="U7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="U8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="U9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="U10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="U11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="U12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="U13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="U14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="U15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="U16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="U2" r:id="rId1"/>
+    <hyperlink ref="U3" r:id="rId2"/>
+    <hyperlink ref="U4" r:id="rId3"/>
+    <hyperlink ref="U5" r:id="rId4"/>
+    <hyperlink ref="U6" r:id="rId5"/>
+    <hyperlink ref="U7" r:id="rId6"/>
+    <hyperlink ref="U8" r:id="rId7"/>
+    <hyperlink ref="U9" r:id="rId8"/>
+    <hyperlink ref="U10" r:id="rId9"/>
+    <hyperlink ref="U11" r:id="rId10"/>
+    <hyperlink ref="U12" r:id="rId11"/>
+    <hyperlink ref="U13" r:id="rId12"/>
+    <hyperlink ref="U14" r:id="rId13"/>
+    <hyperlink ref="U15" r:id="rId14"/>
+    <hyperlink ref="U16" r:id="rId15"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
   <headerFooter>
     <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 EXPLEO Internal</oddFooter>
   </headerFooter>

</xml_diff>